<commit_message>
Some more Product Titel Added
Do Change If Need And make color change to Blue
</commit_message>
<xml_diff>
--- a/electro sports catlog details 2019-2020.xlsx
+++ b/electro sports catlog details 2019-2020.xlsx
@@ -15,8 +15,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Doubt full Product To put Make It Live BCZ of Three Strips In Full Sleeves Copy of Adidas 
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="638">
   <si>
     <t>JS-01</t>
   </si>
@@ -1854,9 +1889,6 @@
     <t xml:space="preserve">Electro Red Colour Jersey with Colour Matching </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro Dark Sky Blu e Colour Jersey </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Black with Pink Matching Jersey </t>
   </si>
   <si>
@@ -1867,13 +1899,79 @@
   </si>
   <si>
     <t>Electro Black Jersey with sublimation Patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro  white Tri Pattern Jersey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro White with matching Pink and Black Jersey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Navy Blue Jersey Matching red and white </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Royal Blue &amp; white matching Jersey </t>
+  </si>
+  <si>
+    <t>Electro Black Jersey with matching Red and grey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Orange Pattern Jersey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Dry-Fit white Jersey with Navy Blue &amp; Orange Matching </t>
+  </si>
+  <si>
+    <t>Electro Dry-fit Navy Blue Jersey with Matching Patterns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro  Black full Sleeves Jersey with Neon Matching </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro yellow full sleeves  Jersey with Matching Patterns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Navy Blue Full Sleeves Jersey with Neon Matching Patterns </t>
+  </si>
+  <si>
+    <t>Electro white full sleeves Jersey with Matching patterns with Three Strips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Orange Full Sleeves Jersey with Navy Blue Matching </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Black Full Sleeves Jersey With Neon Matching </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Dark Sky Blue Colour Jersey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Yellow Full Sleeves with Red &amp; black matching Patterns Made of Nirnal Net Fabric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Light Blue Full Sleeves with Sublimation Sleeves Made of Nirmal Net Fabric </t>
+  </si>
+  <si>
+    <t>Electro Grey Full Sleeves with Red and White Patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Neon Pink Full Sleeves  Jersey with matching Royal Blue  Made of Nirmal Net Fabric </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Black Full Sleeves Jersey With Matching Patterns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Navy Blue  Full Sleeves Jersey With Matching Patterns </t>
+  </si>
+  <si>
+    <t>Electro Orange Full Sleeves Jersey with White &amp; Black Matching Made of Nirmal Net Fabric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1897,8 +1995,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1908,6 +2026,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1985,7 +2109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2018,6 +2142,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2030,10 +2161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2335,11 +2463,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2347,7 +2475,7 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="82.7109375" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
@@ -2434,7 +2562,7 @@
       <c r="C5" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="12" t="s">
         <v>601</v>
       </c>
     </row>
@@ -2448,7 +2576,7 @@
       <c r="C6" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>602</v>
       </c>
     </row>
@@ -2462,7 +2590,7 @@
       <c r="C7" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>603</v>
       </c>
     </row>
@@ -2490,7 +2618,7 @@
       <c r="C9" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="13" t="s">
         <v>605</v>
       </c>
     </row>
@@ -2504,7 +2632,7 @@
       <c r="C10" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="13"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -2516,7 +2644,7 @@
       <c r="C11" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="13" t="s">
         <v>606</v>
       </c>
     </row>
@@ -2530,7 +2658,7 @@
       <c r="C12" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="13" t="s">
         <v>607</v>
       </c>
     </row>
@@ -2544,7 +2672,7 @@
       <c r="C13" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="13" t="s">
         <v>608</v>
       </c>
     </row>
@@ -2558,7 +2686,7 @@
       <c r="C14" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="13" t="s">
         <v>609</v>
       </c>
     </row>
@@ -2572,7 +2700,7 @@
       <c r="C15" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="13" t="s">
         <v>610</v>
       </c>
     </row>
@@ -2586,11 +2714,11 @@
       <c r="C16" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="13" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2600,11 +2728,11 @@
       <c r="C17" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="D17" s="17" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="13" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2614,11 +2742,11 @@
       <c r="C18" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="13" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2628,11 +2756,11 @@
       <c r="C19" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="13" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2642,11 +2770,11 @@
       <c r="C20" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="13" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2656,1544 +2784,1588 @@
       <c r="C21" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="13" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="8" customFormat="1">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:9">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2" t="s">
+      <c r="D24" s="12" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2" t="s">
+      <c r="D25" s="12" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="2" t="s">
+      <c r="D26" s="12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="2" t="s">
+      <c r="D27" s="12" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="2" t="s">
+      <c r="D28" s="12" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="2" t="s">
+      <c r="D29" s="12" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2" t="s">
+      <c r="D30" s="12" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="2" t="s">
+      <c r="D31" s="12" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="D32" s="8"/>
+      <c r="D32" s="12" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="D33" s="8"/>
+        <v>520</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>626</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="D34" s="8"/>
+        <v>521</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="D35" s="8"/>
+        <v>522</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="D36" s="8"/>
+        <v>523</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>629</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="D37" s="8"/>
+        <v>524</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="D38" s="8"/>
+        <v>525</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>632</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="D39" s="8"/>
+        <v>526</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>633</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="D40" s="8"/>
+        <v>527</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>634</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="D41" s="8"/>
+        <v>528</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="D42" s="8"/>
+        <v>529</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="D43" s="8"/>
+        <v>530</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D47" s="8"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D48" s="8"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D60" s="8"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D61" s="8"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D62" s="8"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D67" s="8"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D68" s="8"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D69" s="8"/>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D74" s="8"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D75" s="8"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D76" s="8"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D81" s="8"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>447</v>
+        <v>379</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>569</v>
       </c>
       <c r="D82" s="8"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>570</v>
+        <v>380</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>447</v>
       </c>
       <c r="D83" s="8"/>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D85" s="8"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D86" s="8"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D87" s="8"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D88" s="8"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D89" s="8"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D90" s="8"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D91" s="8"/>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D92" s="8"/>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D93" s="8"/>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D94" s="8"/>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D95" s="8"/>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D96" s="8"/>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D97" s="8"/>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D98" s="8"/>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D99" s="8"/>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D100" s="8"/>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D101" s="8"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D102" s="8"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D103" s="8"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D104" s="8"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D105" s="8"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D106" s="8"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D107" s="8"/>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D108" s="8"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D109" s="8"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>448</v>
+        <v>596</v>
       </c>
       <c r="D110" s="8"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D111" s="8"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D112" s="8"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D113" s="8"/>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D114" s="8"/>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D115" s="8"/>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D116" s="8"/>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D117" s="8"/>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="D117" s="8"/>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B118" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="D118" s="8"/>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D119" s="8"/>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D120" s="8"/>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D121" s="8"/>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D122" s="8"/>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D123" s="8"/>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D124" s="8"/>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D125" s="8"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D126" s="8"/>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D127" s="8"/>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D128" s="8"/>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D129" s="8"/>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D130" s="8"/>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D131" s="8"/>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D132" s="8"/>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D133" s="8"/>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D134" s="8"/>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="D135" s="11" t="s">
-        <v>597</v>
-      </c>
+        <v>472</v>
+      </c>
+      <c r="D135" s="8"/>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="D136" s="8"/>
+        <v>473</v>
+      </c>
+      <c r="D136" s="11" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D137" s="8"/>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D138" s="8"/>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D139" s="8"/>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D140" s="8"/>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D141" s="8"/>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D142" s="8"/>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D143" s="8"/>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D144" s="8"/>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="D145" s="8"/>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B146" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="C145" s="3" t="s">
+      <c r="C146" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="D145" s="8"/>
-    </row>
-    <row r="146" spans="1:9">
-      <c r="A146" s="4" t="s">
+      <c r="D146" s="8"/>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B147" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C147" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="D146" s="8"/>
-    </row>
-    <row r="147" spans="1:9" ht="15" customHeight="1">
-      <c r="A147" s="3" t="s">
+      <c r="D147" s="8"/>
+    </row>
+    <row r="148" spans="1:9" ht="15" customHeight="1">
+      <c r="A148" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B148" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="C147" s="3" t="s">
+      <c r="C148" s="3" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
-      <c r="A148" s="3" t="s">
+    <row r="149" spans="1:9">
+      <c r="A149" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B149" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="C148" s="3" t="s">
+      <c r="C149" s="3" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="149" spans="1:9" ht="15" customHeight="1"/>
-    <row r="156" spans="1:9">
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
-      <c r="F156" s="8"/>
-      <c r="G156" s="8"/>
-      <c r="H156" s="8"/>
-      <c r="I156" s="8"/>
-    </row>
+    <row r="150" spans="1:9" ht="15" customHeight="1"/>
     <row r="157" spans="1:9">
       <c r="B157" s="8"/>
       <c r="C157" s="8"/>
@@ -4284,9 +4456,19 @@
       <c r="H166" s="8"/>
       <c r="I166" s="8"/>
     </row>
+    <row r="167" spans="2:9">
+      <c r="B167" s="8"/>
+      <c r="C167" s="8"/>
+      <c r="D167" s="8"/>
+      <c r="F167" s="8"/>
+      <c r="G167" s="8"/>
+      <c r="H167" s="8"/>
+      <c r="I167" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5174,23 +5356,23 @@
       </c>
     </row>
     <row r="146" spans="1:7">
-      <c r="G146" s="12" t="s">
+      <c r="G146" s="15" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="147" spans="1:7">
-      <c r="G147" s="13"/>
+      <c r="G147" s="16"/>
     </row>
     <row r="148" spans="1:7">
-      <c r="G148" s="12" t="s">
+      <c r="G148" s="15" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="149" spans="1:7">
-      <c r="G149" s="14"/>
+      <c r="G149" s="17"/>
     </row>
     <row r="150" spans="1:7">
-      <c r="G150" s="15"/>
+      <c r="G150" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
One Product Des Update Kindly Check
</commit_message>
<xml_diff>
--- a/electro sports catlog details 2019-2020.xlsx
+++ b/electro sports catlog details 2019-2020.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -22,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D34" authorId="0">
+    <comment ref="D36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="664">
   <si>
     <t>JS-01</t>
   </si>
@@ -2041,6 +2040,13 @@
   </si>
   <si>
     <t xml:space="preserve">Electro super poly Track Suits </t>
+  </si>
+  <si>
+    <t>Get this Tri Colour Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester(100%)
+Sleeve        : Short Hand Sleeve
+Neck            : Colar Neck 
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
 </sst>
 </file>
@@ -2185,7 +2191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2229,6 +2235,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2535,11 +2544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2548,7 +2557,7 @@
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="83.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="68.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
   </cols>
@@ -2582,7 +2591,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="240">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2594,6 +2603,9 @@
       </c>
       <c r="D2" s="10" t="s">
         <v>597</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2955,505 +2967,490 @@
         <v>618</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>620</v>
-      </c>
+    <row r="29" spans="1:9" s="8" customFormat="1">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="8" customFormat="1">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D33" s="12" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:9">
+      <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D34" s="12" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="2" t="s">
+    <row r="35" spans="1:9">
+      <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D35" s="12" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="2" t="s">
+    <row r="36" spans="1:9">
+      <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D36" s="15" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="2" t="s">
+    <row r="37" spans="1:9">
+      <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D37" s="12" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="2" t="s">
+    <row r="38" spans="1:9">
+      <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D38" s="12" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="2" t="s">
+    <row r="39" spans="1:9" s="8" customFormat="1">
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D40" s="12" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="2" t="s">
+    <row r="41" spans="1:9">
+      <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D41" s="12" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="2" t="s">
+    <row r="42" spans="1:9">
+      <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D42" s="12" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="2" t="s">
+    <row r="43" spans="1:9">
+      <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D43" s="12" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="2" t="s">
+    <row r="44" spans="1:9">
+      <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D44" s="12" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="2" t="s">
+    <row r="45" spans="1:9">
+      <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D45" s="12" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="2" t="s">
+    <row r="46" spans="1:9">
+      <c r="A46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D46" s="12" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="2" t="s">
+    <row r="47" spans="1:9" s="8" customFormat="1">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D48" s="12" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="2" t="s">
+    <row r="49" spans="1:9">
+      <c r="A49" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D49" s="12" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="2" t="s">
+    <row r="50" spans="1:9">
+      <c r="A50" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D50" s="12" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="2" t="s">
+    <row r="51" spans="1:9">
+      <c r="A51" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D51" s="12" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="2" t="s">
+    <row r="52" spans="1:9" s="8" customFormat="1">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="D53" s="12" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:9">
       <c r="A54" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="D54" s="12" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:9">
       <c r="A55" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="D55" s="12" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="D56" s="12" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:9">
       <c r="A57" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D57" s="12" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:9">
       <c r="A58" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C63" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="D58" s="12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D59" s="12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="D62" s="12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>550</v>
       </c>
       <c r="D63" s="12" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:9">
       <c r="A64" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="D64" s="12" t="s">
         <v>645</v>
@@ -3461,13 +3458,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="D65" s="12" t="s">
         <v>645</v>
@@ -3475,13 +3472,13 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="D66" s="12" t="s">
         <v>645</v>
@@ -3489,13 +3486,13 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="D67" s="12" t="s">
         <v>645</v>
@@ -3503,13 +3500,13 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="D68" s="12" t="s">
         <v>645</v>
@@ -3517,13 +3514,13 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="D69" s="12" t="s">
         <v>645</v>
@@ -3531,13 +3528,13 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="D70" s="12" t="s">
         <v>645</v>
@@ -3545,13 +3542,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="D71" s="12" t="s">
         <v>645</v>
@@ -3559,13 +3556,13 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D72" s="12" t="s">
         <v>645</v>
@@ -3573,13 +3570,13 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="D73" s="12" t="s">
         <v>645</v>
@@ -3587,13 +3584,13 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="D74" s="12" t="s">
         <v>645</v>
@@ -3601,13 +3598,13 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="D75" s="12" t="s">
         <v>645</v>
@@ -3615,13 +3612,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="D76" s="12" t="s">
         <v>645</v>
@@ -3629,13 +3626,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="D77" s="12" t="s">
         <v>645</v>
@@ -3643,13 +3640,13 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D78" s="12" t="s">
         <v>645</v>
@@ -3657,13 +3654,13 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="D79" s="12" t="s">
         <v>645</v>
@@ -3671,1081 +3668,1239 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D80" s="12" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:9">
       <c r="A81" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="D81" s="12" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:9">
       <c r="A82" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="D82" s="12" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:9">
       <c r="A83" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="8" customFormat="1">
+      <c r="A88" s="14"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B89" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="C83" s="9" t="s">
+      <c r="C89" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="D83" s="16"/>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="2" t="s">
+      <c r="D89" s="16"/>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="D84" s="12" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="D85" s="12" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="D88" s="12" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="D89" s="12" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>576</v>
       </c>
       <c r="D90" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:9">
       <c r="A91" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="D91" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:9">
       <c r="A92" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="D92" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:9">
       <c r="A93" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="D93" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:9">
       <c r="A94" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="D94" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:9">
       <c r="A95" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="D95" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:9">
       <c r="A96" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="D96" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:9">
       <c r="A97" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D97" s="12" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:9">
       <c r="A98" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" s="8" customFormat="1">
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="C105" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="D105" s="12" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
+    <row r="106" spans="1:9">
+      <c r="A106" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C106" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="D99" s="12" t="s">
+      <c r="D106" s="12" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2" t="s">
+    <row r="107" spans="1:9">
+      <c r="A107" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B107" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C107" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D107" s="12" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="2" t="s">
+    <row r="108" spans="1:9">
+      <c r="A108" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B108" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C101" s="2" t="s">
+      <c r="C108" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="D101" s="12" t="s">
+      <c r="D108" s="12" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" s="2" t="s">
+    <row r="109" spans="1:9">
+      <c r="A109" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B109" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="C102" s="2" t="s">
+      <c r="C109" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="D102" s="12" t="s">
+      <c r="D109" s="12" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" s="2" t="s">
+    <row r="110" spans="1:9">
+      <c r="A110" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B110" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="C103" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D110" s="12" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="2" t="s">
+    <row r="111" spans="1:9">
+      <c r="A111" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B111" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="C104" s="2" t="s">
+      <c r="C111" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D104" s="12" t="s">
+      <c r="D111" s="12" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="2" t="s">
+    <row r="112" spans="1:9" s="8" customFormat="1">
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B113" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="C105" s="2" t="s">
+      <c r="C113" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="D105" s="12" t="s">
+      <c r="D113" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="2" t="s">
+    <row r="114" spans="1:9">
+      <c r="A114" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B114" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C114" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="D106" s="12" t="s">
+      <c r="D114" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="2" t="s">
+    <row r="115" spans="1:9">
+      <c r="A115" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B115" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D115" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="2" t="s">
+    <row r="116" spans="1:9">
+      <c r="A116" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B116" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C108" s="2" t="s">
+      <c r="C116" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D116" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
-      <c r="A109" s="2" t="s">
+    <row r="117" spans="1:9" s="8" customFormat="1">
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B118" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="C109" s="2" t="s">
+      <c r="C118" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D118" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="2" t="s">
+    <row r="119" spans="1:9">
+      <c r="A119" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B119" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="C110" s="2" t="s">
+      <c r="C119" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="D110" s="12" t="s">
+      <c r="D119" s="12" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="2" t="s">
+    <row r="120" spans="1:9" s="8" customFormat="1">
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B121" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="D111" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D112" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="D113" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="D114" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D115" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D116" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="D117" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D118" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="D119" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4">
-      <c r="A120" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>457</v>
-      </c>
-      <c r="D120" s="12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4">
-      <c r="A121" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>458</v>
       </c>
       <c r="D121" s="12" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
-      <c r="A122" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B122" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>459</v>
+    <row r="122" spans="1:9">
+      <c r="A122" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>449</v>
       </c>
       <c r="D122" s="12" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>460</v>
+    <row r="123" spans="1:9">
+      <c r="A123" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>450</v>
       </c>
       <c r="D123" s="12" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="3" t="s">
+    <row r="124" spans="1:9">
+      <c r="A124" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="D130" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D131" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D132" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="D133" s="12" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="A134" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B134" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="C124" s="3" t="s">
+      <c r="C134" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="D124" s="12" t="s">
+      <c r="D134" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
-      <c r="A125" s="3" t="s">
+    <row r="135" spans="1:9">
+      <c r="A135" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B135" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C135" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="D125" s="12" t="s">
+      <c r="D135" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
-      <c r="A126" s="3" t="s">
+    <row r="136" spans="1:9">
+      <c r="A136" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B126" s="3" t="s">
+      <c r="B136" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="C136" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="D126" s="12" t="s">
+      <c r="D136" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
-      <c r="A127" s="3" t="s">
+    <row r="137" spans="1:9">
+      <c r="A137" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="B137" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="C127" s="3" t="s">
+      <c r="C137" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="D127" s="12" t="s">
+      <c r="D137" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
-      <c r="A128" s="3" t="s">
+    <row r="138" spans="1:9">
+      <c r="A138" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B128" s="3" t="s">
+      <c r="B138" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="C128" s="3" t="s">
+      <c r="C138" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="D128" s="12" t="s">
+      <c r="D138" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
-      <c r="A129" s="3" t="s">
+    <row r="139" spans="1:9">
+      <c r="A139" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B129" s="3" t="s">
+      <c r="B139" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="C129" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="D129" s="12" t="s">
+      <c r="D139" s="12" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
-      <c r="A130" s="3" t="s">
+    <row r="140" spans="1:9" s="8" customFormat="1">
+      <c r="A140" s="14"/>
+      <c r="B140" s="14"/>
+      <c r="C140" s="14"/>
+      <c r="D140" s="14"/>
+      <c r="E140" s="14"/>
+      <c r="F140" s="14"/>
+      <c r="G140" s="14"/>
+      <c r="H140" s="14"/>
+      <c r="I140" s="14"/>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="B141" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="C130" s="3" t="s">
+      <c r="C141" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="D130" s="12" t="s">
+      <c r="D141" s="12" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
-      <c r="A131" s="3" t="s">
+    <row r="142" spans="1:9">
+      <c r="A142" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B131" s="3" t="s">
+      <c r="B142" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="C142" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="D131" s="12" t="s">
+      <c r="D142" s="12" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
-      <c r="A132" s="3" t="s">
+    <row r="143" spans="1:9">
+      <c r="A143" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B143" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="C132" s="3" t="s">
+      <c r="C143" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="D132" s="12" t="s">
+      <c r="D143" s="12" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
-      <c r="A133" s="3" t="s">
+    <row r="144" spans="1:9">
+      <c r="A144" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B133" s="3" t="s">
+      <c r="B144" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="C133" s="3" t="s">
+      <c r="C144" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="D133" s="12" t="s">
+      <c r="D144" s="12" t="s">
         <v>657</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4">
-      <c r="A134" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="D134" s="12" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4">
-      <c r="A135" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B135" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>472</v>
-      </c>
-      <c r="D135" s="12" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4">
-      <c r="A136" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="D136" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4">
-      <c r="A137" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B137" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="D137" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4">
-      <c r="A138" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>475</v>
-      </c>
-      <c r="D138" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>476</v>
-      </c>
-      <c r="D139" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4">
-      <c r="A140" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B140" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="D140" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4">
-      <c r="A141" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="D141" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B142" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="D142" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4">
-      <c r="A143" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B143" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="D143" s="11" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4">
-      <c r="A144" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B144" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="D144" s="11" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="145" spans="1:9">
       <c r="A145" s="3" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="D145" s="11" t="s">
-        <v>660</v>
+        <v>471</v>
+      </c>
+      <c r="D145" s="12" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="3" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>443</v>
+        <v>432</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="D146" s="11" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9">
-      <c r="A147" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>444</v>
-      </c>
-      <c r="C147" s="4" t="s">
-        <v>484</v>
-      </c>
-      <c r="D147" s="11" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" ht="15" customHeight="1">
+        <v>472</v>
+      </c>
+      <c r="D146" s="12" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" s="8" customFormat="1">
+      <c r="A147" s="14"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="14"/>
+      <c r="D147" s="14"/>
+      <c r="E147" s="14"/>
+      <c r="F147" s="14"/>
+      <c r="G147" s="14"/>
+      <c r="H147" s="14"/>
+      <c r="I147" s="14"/>
+    </row>
+    <row r="148" spans="1:9">
       <c r="A148" s="3" t="s">
-        <v>504</v>
+        <v>133</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>505</v>
+        <v>433</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>506</v>
+        <v>473</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="149" spans="1:9">
       <c r="A149" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="D149" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="D150" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="A151" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D151" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="D152" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="A153" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D153" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="A154" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D154" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9">
+      <c r="A155" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="D155" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9">
+      <c r="A156" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="D156" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="D157" s="11" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" s="8" customFormat="1">
+      <c r="A158" s="14"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="14"/>
+      <c r="D158" s="14"/>
+      <c r="E158" s="14"/>
+      <c r="F158" s="14"/>
+      <c r="G158" s="14"/>
+      <c r="H158" s="14"/>
+      <c r="I158" s="14"/>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="A159" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="A160" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C160" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="D160" s="11" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="15" customHeight="1">
+      <c r="A161" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="D161" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9">
+      <c r="A162" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B162" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="C149" s="3" t="s">
+      <c r="C162" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="D149" s="11" t="s">
+      <c r="D162" s="11" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="150" spans="1:9" ht="15" customHeight="1"/>
-    <row r="157" spans="1:9">
-      <c r="B157" s="8"/>
-      <c r="C157" s="8"/>
-      <c r="D157" s="8"/>
-      <c r="F157" s="8"/>
-      <c r="G157" s="8"/>
-      <c r="H157" s="8"/>
-      <c r="I157" s="8"/>
-    </row>
-    <row r="158" spans="1:9">
-      <c r="B158" s="8"/>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
-      <c r="F158" s="8"/>
-      <c r="G158" s="8"/>
-      <c r="H158" s="8"/>
-      <c r="I158" s="8"/>
-    </row>
-    <row r="159" spans="1:9">
-      <c r="B159" s="8"/>
-      <c r="C159" s="8"/>
-      <c r="D159" s="8"/>
-      <c r="F159" s="8"/>
-      <c r="G159" s="8"/>
-      <c r="H159" s="8"/>
-      <c r="I159" s="8"/>
-    </row>
-    <row r="160" spans="1:9">
-      <c r="B160" s="8"/>
-      <c r="C160" s="8"/>
-      <c r="D160" s="8"/>
-      <c r="F160" s="8"/>
-      <c r="G160" s="8"/>
-      <c r="H160" s="8"/>
-      <c r="I160" s="8"/>
-    </row>
-    <row r="161" spans="2:9">
-      <c r="B161" s="8"/>
-      <c r="C161" s="8"/>
-      <c r="D161" s="8"/>
-      <c r="F161" s="8"/>
-      <c r="G161" s="8"/>
-      <c r="H161" s="8"/>
-      <c r="I161" s="8"/>
-    </row>
-    <row r="162" spans="2:9">
-      <c r="B162" s="8"/>
-      <c r="C162" s="8"/>
-      <c r="D162" s="8"/>
-      <c r="F162" s="8"/>
-      <c r="G162" s="8"/>
-      <c r="H162" s="8"/>
-      <c r="I162" s="8"/>
-    </row>
-    <row r="163" spans="2:9">
-      <c r="B163" s="8"/>
-      <c r="C163" s="8"/>
-      <c r="D163" s="8"/>
-      <c r="F163" s="8"/>
-      <c r="G163" s="8"/>
-      <c r="H163" s="8"/>
-      <c r="I163" s="8"/>
-    </row>
-    <row r="164" spans="2:9">
-      <c r="B164" s="8"/>
-      <c r="C164" s="8"/>
-      <c r="D164" s="8"/>
-      <c r="F164" s="8"/>
-      <c r="G164" s="8"/>
-      <c r="H164" s="8"/>
-      <c r="I164" s="8"/>
-    </row>
-    <row r="165" spans="2:9">
-      <c r="B165" s="8"/>
-      <c r="C165" s="8"/>
-      <c r="D165" s="8"/>
-      <c r="F165" s="8"/>
-      <c r="G165" s="8"/>
-      <c r="H165" s="8"/>
-      <c r="I165" s="8"/>
-    </row>
-    <row r="166" spans="2:9">
-      <c r="B166" s="8"/>
-      <c r="C166" s="8"/>
-      <c r="D166" s="8"/>
-      <c r="F166" s="8"/>
-      <c r="G166" s="8"/>
-      <c r="H166" s="8"/>
-      <c r="I166" s="8"/>
-    </row>
-    <row r="167" spans="2:9">
-      <c r="B167" s="8"/>
-      <c r="C167" s="8"/>
-      <c r="D167" s="8"/>
-      <c r="F167" s="8"/>
-      <c r="G167" s="8"/>
-      <c r="H167" s="8"/>
-      <c r="I167" s="8"/>
+    <row r="163" spans="1:9" ht="15" customHeight="1"/>
+    <row r="170" spans="1:9">
+      <c r="B170" s="8"/>
+      <c r="C170" s="8"/>
+      <c r="D170" s="8"/>
+      <c r="F170" s="8"/>
+      <c r="G170" s="8"/>
+      <c r="H170" s="8"/>
+      <c r="I170" s="8"/>
+    </row>
+    <row r="171" spans="1:9">
+      <c r="B171" s="8"/>
+      <c r="C171" s="8"/>
+      <c r="D171" s="8"/>
+      <c r="F171" s="8"/>
+      <c r="G171" s="8"/>
+      <c r="H171" s="8"/>
+      <c r="I171" s="8"/>
+    </row>
+    <row r="172" spans="1:9">
+      <c r="B172" s="8"/>
+      <c r="C172" s="8"/>
+      <c r="D172" s="8"/>
+      <c r="F172" s="8"/>
+      <c r="G172" s="8"/>
+      <c r="H172" s="8"/>
+      <c r="I172" s="8"/>
+    </row>
+    <row r="173" spans="1:9">
+      <c r="B173" s="8"/>
+      <c r="C173" s="8"/>
+      <c r="D173" s="8"/>
+      <c r="F173" s="8"/>
+      <c r="G173" s="8"/>
+      <c r="H173" s="8"/>
+      <c r="I173" s="8"/>
+    </row>
+    <row r="174" spans="1:9">
+      <c r="B174" s="8"/>
+      <c r="C174" s="8"/>
+      <c r="D174" s="8"/>
+      <c r="F174" s="8"/>
+      <c r="G174" s="8"/>
+      <c r="H174" s="8"/>
+      <c r="I174" s="8"/>
+    </row>
+    <row r="175" spans="1:9">
+      <c r="B175" s="8"/>
+      <c r="C175" s="8"/>
+      <c r="D175" s="8"/>
+      <c r="F175" s="8"/>
+      <c r="G175" s="8"/>
+      <c r="H175" s="8"/>
+      <c r="I175" s="8"/>
+    </row>
+    <row r="176" spans="1:9">
+      <c r="B176" s="8"/>
+      <c r="C176" s="8"/>
+      <c r="D176" s="8"/>
+      <c r="F176" s="8"/>
+      <c r="G176" s="8"/>
+      <c r="H176" s="8"/>
+      <c r="I176" s="8"/>
+    </row>
+    <row r="177" spans="2:9">
+      <c r="B177" s="8"/>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
+      <c r="F177" s="8"/>
+      <c r="G177" s="8"/>
+      <c r="H177" s="8"/>
+      <c r="I177" s="8"/>
+    </row>
+    <row r="178" spans="2:9">
+      <c r="B178" s="8"/>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
+      <c r="F178" s="8"/>
+      <c r="G178" s="8"/>
+      <c r="H178" s="8"/>
+      <c r="I178" s="8"/>
+    </row>
+    <row r="179" spans="2:9">
+      <c r="B179" s="8"/>
+      <c r="C179" s="8"/>
+      <c r="D179" s="8"/>
+      <c r="F179" s="8"/>
+      <c r="G179" s="8"/>
+      <c r="H179" s="8"/>
+      <c r="I179" s="8"/>
+    </row>
+    <row r="180" spans="2:9">
+      <c r="B180" s="8"/>
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+      <c r="F180" s="8"/>
+      <c r="G180" s="8"/>
+      <c r="H180" s="8"/>
+      <c r="I180" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5638,23 +5793,23 @@
       </c>
     </row>
     <row r="146" spans="1:7">
-      <c r="G146" s="17" t="s">
+      <c r="G146" s="18" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="147" spans="1:7">
-      <c r="G147" s="18"/>
+      <c r="G147" s="19"/>
     </row>
     <row r="148" spans="1:7">
-      <c r="G148" s="17" t="s">
+      <c r="G148" s="18" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="149" spans="1:7">
-      <c r="G149" s="19"/>
+      <c r="G149" s="20"/>
     </row>
     <row r="150" spans="1:7">
-      <c r="G150" s="20"/>
+      <c r="G150" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
please add colour details of title in brackets
</commit_message>
<xml_diff>
--- a/electro sports catlog details 2019-2020.xlsx
+++ b/electro sports catlog details 2019-2020.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{713BA3CC-01AD-4D8C-A403-7F23D16FCE5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="electro_Sports " sheetId="1" r:id="rId1"/>
@@ -16,12 +17,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D36" authorId="0">
+    <comment ref="D36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2042,18 +2043,18 @@
     <t xml:space="preserve">Electro super poly Track Suits </t>
   </si>
   <si>
-    <t>Get this Tri Colour Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+    <t>Get this Tri Colour Jersey from Electro.Electro Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat. This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc.
 Fabric          : Polyester(100%)
 Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
-Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+Neck            : Collar Neck 
+Note : Now You Can Customize This T-shirt As Per Your Requirement. Please revert us back with your query on contact page.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2256,6 +2257,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2302,7 +2311,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2334,9 +2343,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2368,6 +2395,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2543,26 +2588,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" customWidth="1"/>
-    <col min="5" max="5" width="68.140625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="83.6640625" customWidth="1"/>
+    <col min="5" max="5" width="68.109375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>145</v>
       </c>
@@ -2591,7 +2636,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="240">
+    <row r="2" spans="1:9" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2608,7 +2653,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -2622,7 +2667,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2636,7 +2681,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2650,7 +2695,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2664,7 +2709,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -2678,7 +2723,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -2692,7 +2737,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -2706,7 +2751,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2718,7 +2763,7 @@
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2732,7 +2777,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2746,7 +2791,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -2760,7 +2805,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -2774,7 +2819,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -2788,7 +2833,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -2802,7 +2847,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2816,7 +2861,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2830,7 +2875,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2844,7 +2889,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2858,7 +2903,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -2872,7 +2917,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="8" customFormat="1">
+    <row r="22" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2883,7 +2928,7 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
@@ -2897,7 +2942,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -2911,7 +2956,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -2925,7 +2970,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
@@ -2939,7 +2984,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2953,7 +2998,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2967,7 +3012,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="8" customFormat="1">
+    <row r="29" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
@@ -2978,7 +3023,7 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2992,7 +3037,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -3006,7 +3051,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="8" customFormat="1">
+    <row r="32" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="14"/>
       <c r="C32" s="14"/>
@@ -3017,7 +3062,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -3031,7 +3076,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -3045,7 +3090,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>30</v>
       </c>
@@ -3059,7 +3104,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>31</v>
       </c>
@@ -3073,7 +3118,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>32</v>
       </c>
@@ -3087,7 +3132,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
@@ -3101,7 +3146,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="8" customFormat="1">
+    <row r="39" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -3112,7 +3157,7 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
@@ -3126,7 +3171,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
@@ -3140,7 +3185,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>36</v>
       </c>
@@ -3154,7 +3199,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>37</v>
       </c>
@@ -3168,7 +3213,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
@@ -3182,7 +3227,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>39</v>
       </c>
@@ -3196,7 +3241,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>40</v>
       </c>
@@ -3210,7 +3255,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="47" spans="1:9" s="8" customFormat="1">
+    <row r="47" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="B47" s="14"/>
       <c r="C47" s="14"/>
@@ -3221,7 +3266,7 @@
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>41</v>
       </c>
@@ -3235,7 +3280,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>42</v>
       </c>
@@ -3249,7 +3294,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>43</v>
       </c>
@@ -3263,7 +3308,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>44</v>
       </c>
@@ -3277,7 +3322,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="8" customFormat="1">
+    <row r="52" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14"/>
       <c r="B52" s="14"/>
       <c r="C52" s="14"/>
@@ -3288,7 +3333,7 @@
       <c r="H52" s="14"/>
       <c r="I52" s="14"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>45</v>
       </c>
@@ -3302,7 +3347,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>46</v>
       </c>
@@ -3316,7 +3361,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>47</v>
       </c>
@@ -3330,7 +3375,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>48</v>
       </c>
@@ -3344,7 +3389,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>49</v>
       </c>
@@ -3358,7 +3403,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>50</v>
       </c>
@@ -3372,7 +3417,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>51</v>
       </c>
@@ -3386,7 +3431,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>52</v>
       </c>
@@ -3400,7 +3445,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>53</v>
       </c>
@@ -3414,7 +3459,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>54</v>
       </c>
@@ -3428,7 +3473,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>55</v>
       </c>
@@ -3442,7 +3487,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>56</v>
       </c>
@@ -3456,7 +3501,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>57</v>
       </c>
@@ -3470,7 +3515,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>58</v>
       </c>
@@ -3484,7 +3529,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>59</v>
       </c>
@@ -3498,7 +3543,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>60</v>
       </c>
@@ -3512,7 +3557,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>61</v>
       </c>
@@ -3526,7 +3571,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>62</v>
       </c>
@@ -3540,7 +3585,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>63</v>
       </c>
@@ -3554,7 +3599,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
@@ -3568,7 +3613,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
@@ -3582,7 +3627,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>66</v>
       </c>
@@ -3596,7 +3641,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>67</v>
       </c>
@@ -3610,7 +3655,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>68</v>
       </c>
@@ -3624,7 +3669,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>69</v>
       </c>
@@ -3638,7 +3683,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
@@ -3652,7 +3697,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>71</v>
       </c>
@@ -3666,7 +3711,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>72</v>
       </c>
@@ -3680,7 +3725,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="81" spans="1:9">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>73</v>
       </c>
@@ -3694,7 +3739,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="82" spans="1:9">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>74</v>
       </c>
@@ -3708,7 +3753,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="83" spans="1:9">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>75</v>
       </c>
@@ -3722,7 +3767,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="84" spans="1:9">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>76</v>
       </c>
@@ -3736,7 +3781,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="85" spans="1:9">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>77</v>
       </c>
@@ -3750,7 +3795,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="86" spans="1:9">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>78</v>
       </c>
@@ -3764,7 +3809,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>79</v>
       </c>
@@ -3778,7 +3823,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="88" spans="1:9" s="8" customFormat="1">
+    <row r="88" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="14"/>
       <c r="B88" s="14"/>
       <c r="C88" s="14"/>
@@ -3789,7 +3834,7 @@
       <c r="H88" s="14"/>
       <c r="I88" s="14"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>80</v>
       </c>
@@ -3801,7 +3846,7 @@
       </c>
       <c r="D89" s="16"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>81</v>
       </c>
@@ -3815,7 +3860,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>82</v>
       </c>
@@ -3829,7 +3874,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>83</v>
       </c>
@@ -3843,7 +3888,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>84</v>
       </c>
@@ -3857,7 +3902,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>85</v>
       </c>
@@ -3871,7 +3916,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>86</v>
       </c>
@@ -3885,7 +3930,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>87</v>
       </c>
@@ -3899,7 +3944,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>88</v>
       </c>
@@ -3913,7 +3958,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>89</v>
       </c>
@@ -3927,7 +3972,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>90</v>
       </c>
@@ -3941,7 +3986,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>91</v>
       </c>
@@ -3955,7 +4000,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>92</v>
       </c>
@@ -3969,7 +4014,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>93</v>
       </c>
@@ -3983,7 +4028,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>94</v>
       </c>
@@ -3997,7 +4042,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="104" spans="1:9" s="8" customFormat="1">
+    <row r="104" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="14"/>
       <c r="B104" s="14"/>
       <c r="C104" s="14"/>
@@ -4008,7 +4053,7 @@
       <c r="H104" s="14"/>
       <c r="I104" s="14"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>95</v>
       </c>
@@ -4022,7 +4067,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>96</v>
       </c>
@@ -4036,7 +4081,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>97</v>
       </c>
@@ -4050,7 +4095,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>98</v>
       </c>
@@ -4064,7 +4109,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>99</v>
       </c>
@@ -4078,7 +4123,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>100</v>
       </c>
@@ -4092,7 +4137,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>101</v>
       </c>
@@ -4106,7 +4151,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="112" spans="1:9" s="8" customFormat="1">
+    <row r="112" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="14"/>
       <c r="B112" s="14"/>
       <c r="C112" s="14"/>
@@ -4117,7 +4162,7 @@
       <c r="H112" s="14"/>
       <c r="I112" s="14"/>
     </row>
-    <row r="113" spans="1:9">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>102</v>
       </c>
@@ -4131,7 +4176,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>103</v>
       </c>
@@ -4145,7 +4190,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>104</v>
       </c>
@@ -4159,7 +4204,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>105</v>
       </c>
@@ -4173,7 +4218,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="117" spans="1:9" s="8" customFormat="1">
+    <row r="117" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
       <c r="C117" s="14"/>
@@ -4184,7 +4229,7 @@
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>106</v>
       </c>
@@ -4198,7 +4243,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="119" spans="1:9">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>107</v>
       </c>
@@ -4212,7 +4257,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="120" spans="1:9" s="8" customFormat="1">
+    <row r="120" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="14"/>
       <c r="B120" s="14"/>
       <c r="C120" s="14"/>
@@ -4223,7 +4268,7 @@
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>108</v>
       </c>
@@ -4237,7 +4282,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>109</v>
       </c>
@@ -4251,7 +4296,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>110</v>
       </c>
@@ -4265,7 +4310,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>111</v>
       </c>
@@ -4279,7 +4324,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>112</v>
       </c>
@@ -4293,7 +4338,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>113</v>
       </c>
@@ -4307,7 +4352,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>114</v>
       </c>
@@ -4321,7 +4366,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>115</v>
       </c>
@@ -4335,7 +4380,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>116</v>
       </c>
@@ -4349,7 +4394,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>117</v>
       </c>
@@ -4363,7 +4408,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>118</v>
       </c>
@@ -4377,7 +4422,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>119</v>
       </c>
@@ -4391,7 +4436,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>120</v>
       </c>
@@ -4405,7 +4450,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>121</v>
       </c>
@@ -4419,7 +4464,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>122</v>
       </c>
@@ -4433,7 +4478,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>123</v>
       </c>
@@ -4447,7 +4492,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="137" spans="1:9">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>124</v>
       </c>
@@ -4461,7 +4506,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>125</v>
       </c>
@@ -4475,7 +4520,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>126</v>
       </c>
@@ -4489,7 +4534,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="140" spans="1:9" s="8" customFormat="1">
+    <row r="140" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="14"/>
       <c r="B140" s="14"/>
       <c r="C140" s="14"/>
@@ -4500,7 +4545,7 @@
       <c r="H140" s="14"/>
       <c r="I140" s="14"/>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>127</v>
       </c>
@@ -4514,7 +4559,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>128</v>
       </c>
@@ -4528,7 +4573,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="143" spans="1:9">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>129</v>
       </c>
@@ -4542,7 +4587,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="144" spans="1:9">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>130</v>
       </c>
@@ -4556,7 +4601,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="145" spans="1:9">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>131</v>
       </c>
@@ -4570,7 +4615,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>132</v>
       </c>
@@ -4584,7 +4629,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="147" spans="1:9" s="8" customFormat="1">
+    <row r="147" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="14"/>
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
@@ -4595,7 +4640,7 @@
       <c r="H147" s="14"/>
       <c r="I147" s="14"/>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>133</v>
       </c>
@@ -4609,7 +4654,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="149" spans="1:9">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>134</v>
       </c>
@@ -4623,7 +4668,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>135</v>
       </c>
@@ -4637,7 +4682,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="151" spans="1:9">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>136</v>
       </c>
@@ -4651,7 +4696,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
         <v>137</v>
       </c>
@@ -4665,7 +4710,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="153" spans="1:9">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>138</v>
       </c>
@@ -4679,7 +4724,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="154" spans="1:9">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>139</v>
       </c>
@@ -4693,7 +4738,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
         <v>140</v>
       </c>
@@ -4707,7 +4752,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="156" spans="1:9">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
         <v>141</v>
       </c>
@@ -4721,7 +4766,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="157" spans="1:9">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>142</v>
       </c>
@@ -4735,7 +4780,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="158" spans="1:9" s="8" customFormat="1">
+    <row r="158" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="14"/>
       <c r="B158" s="14"/>
       <c r="C158" s="14"/>
@@ -4746,7 +4791,7 @@
       <c r="H158" s="14"/>
       <c r="I158" s="14"/>
     </row>
-    <row r="159" spans="1:9">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>143</v>
       </c>
@@ -4760,7 +4805,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="160" spans="1:9">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>144</v>
       </c>
@@ -4774,7 +4819,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="15" customHeight="1">
+    <row r="161" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>504</v>
       </c>
@@ -4788,7 +4833,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="162" spans="1:9">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>507</v>
       </c>
@@ -4802,8 +4847,8 @@
         <v>662</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="15" customHeight="1"/>
-    <row r="170" spans="1:9">
+    <row r="163" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
       <c r="D170" s="8"/>
@@ -4812,7 +4857,7 @@
       <c r="H170" s="8"/>
       <c r="I170" s="8"/>
     </row>
-    <row r="171" spans="1:9">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
       <c r="D171" s="8"/>
@@ -4821,7 +4866,7 @@
       <c r="H171" s="8"/>
       <c r="I171" s="8"/>
     </row>
-    <row r="172" spans="1:9">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
       <c r="D172" s="8"/>
@@ -4830,7 +4875,7 @@
       <c r="H172" s="8"/>
       <c r="I172" s="8"/>
     </row>
-    <row r="173" spans="1:9">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
       <c r="D173" s="8"/>
@@ -4839,7 +4884,7 @@
       <c r="H173" s="8"/>
       <c r="I173" s="8"/>
     </row>
-    <row r="174" spans="1:9">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
       <c r="D174" s="8"/>
@@ -4848,7 +4893,7 @@
       <c r="H174" s="8"/>
       <c r="I174" s="8"/>
     </row>
-    <row r="175" spans="1:9">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
       <c r="D175" s="8"/>
@@ -4857,7 +4902,7 @@
       <c r="H175" s="8"/>
       <c r="I175" s="8"/>
     </row>
-    <row r="176" spans="1:9">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
       <c r="D176" s="8"/>
@@ -4866,7 +4911,7 @@
       <c r="H176" s="8"/>
       <c r="I176" s="8"/>
     </row>
-    <row r="177" spans="2:9">
+    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
       <c r="D177" s="8"/>
@@ -4875,7 +4920,7 @@
       <c r="H177" s="8"/>
       <c r="I177" s="8"/>
     </row>
-    <row r="178" spans="2:9">
+    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
       <c r="D178" s="8"/>
@@ -4884,7 +4929,7 @@
       <c r="H178" s="8"/>
       <c r="I178" s="8"/>
     </row>
-    <row r="179" spans="2:9">
+    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
       <c r="D179" s="8"/>
@@ -4893,7 +4938,7 @@
       <c r="H179" s="8"/>
       <c r="I179" s="8"/>
     </row>
-    <row r="180" spans="2:9">
+    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
       <c r="D180" s="8"/>
@@ -4910,905 +4955,905 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView topLeftCell="A123" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="G1" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="G2" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="G3" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="G4" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="G5" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="G6" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="G7" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="G8" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="G9" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="G10" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="G11" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="G13" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="G14" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="G15" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="G16" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="G17" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="G18" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="G19" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="G20" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="G21" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="G22" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="G23" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="G24" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="G25" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="G26" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="G27" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="G28" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="G29" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="G30" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="G31" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="G32" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="G33" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="G34" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="G35" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="G36" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="G37" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="G38" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="G39" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="G40" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="G41" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="G42" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="G43" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="G44" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="G45" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="G46" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="G47" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="G48" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="G49" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="G50" s="2" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="G51" s="2" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="G52" s="2" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="G53" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="G54" s="2" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="G55" s="2" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="G56" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="G57" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="G58" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="G59" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="G60" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="G61" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="G62" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="G63" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="G64" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="G65" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="G66" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="G67" s="2" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="G68" s="2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="G69" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="G70" s="2" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="G71" s="2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="G72" s="2" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="G73" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="G74" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="G75" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="G76" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="G77" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="G78" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="G79" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="G80" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="G81" s="2" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="G82" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="G83" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="G84" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="G85" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="G86" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="G87" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="G88" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="G89" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="G90" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="G91" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="G92" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="G93" s="2" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="G94" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="G95" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="G96" s="2" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="G97" s="2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="G98" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="G99" s="2" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="G100" s="2" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="G101" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="G102" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="G103" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="G104" s="2" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="G105" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="G106" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="G107" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="G108" s="2" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="G109" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="G110" s="2" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="G111" s="2" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="G112" s="2" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="G113" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="G114" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="G115" s="2" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="G116" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="G117" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="G118" s="3" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="G119" s="3" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="G120" s="3" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="G121" s="3" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="G122" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="G123" s="3" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="G124" s="3" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="G125" s="3" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="G126" s="3" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="G127" s="3" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="G128" s="3" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="G129" s="3" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="G130" s="3" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="G131" s="3" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="G132" s="3" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="G133" s="3" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="3"/>
       <c r="G134" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="3"/>
       <c r="G135" s="3" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="3"/>
       <c r="G136" s="3" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="3"/>
       <c r="G137" s="3" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="3"/>
       <c r="G138" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="3"/>
       <c r="G139" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="3"/>
       <c r="G140" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="3"/>
       <c r="G141" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="3"/>
       <c r="G142" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="3"/>
       <c r="G143" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="3"/>
       <c r="G144" s="3" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="145" spans="1:7">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="4"/>
       <c r="G145" s="4" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G146" s="18" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G147" s="19"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G148" s="18" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G149" s="20"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G150" s="21"/>
     </row>
   </sheetData>
@@ -5821,12 +5866,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Product Detail almost Completed
</commit_message>
<xml_diff>
--- a/electro sports catlog details 2019-2020.xlsx
+++ b/electro sports catlog details 2019-2020.xlsx
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="697">
   <si>
     <t>JS-01</t>
   </si>
@@ -1847,66 +1847,30 @@
     <t>Electro Tri Colour Jersey With Collar</t>
   </si>
   <si>
-    <t>Electro Black With Neon Pattern Jersey</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Yellow Mix Colour Patch Jersey </t>
   </si>
   <si>
     <t xml:space="preserve">Electro Royal Blue Jersey </t>
   </si>
   <si>
-    <t>Electro Tri Colour Jersey With Sublimation Print</t>
-  </si>
-  <si>
-    <t>Electro Navy blue  With Neon Pattern Jersey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electro Black Jersey with Neon matching </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Yellow matching Grey Jersey </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro white with Light Blue Matching Jersey </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Orange and White matching Jersey </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro Royal Blue with white &amp; Black Matching </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Red Colour Jersey with Colour Matching </t>
   </si>
   <si>
     <t xml:space="preserve">Electro Black with Pink Matching Jersey </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro white white matching Orange and Blue Jersey </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electro Sky blue Jersey with macthing colour </t>
-  </si>
-  <si>
-    <t>Electro Black Jersey with sublimation Patch</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro  white Tri Pattern Jersey </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro White with matching Pink and Black Jersey </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electro Navy Blue Jersey Matching red and white </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Royal Blue &amp; white matching Jersey </t>
   </si>
   <si>
-    <t>Electro Black Jersey with matching Red and grey</t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Orange Pattern Jersey </t>
   </si>
   <si>
@@ -1916,36 +1880,15 @@
     <t>Electro Dry-fit Navy Blue Jersey with Matching Patterns</t>
   </si>
   <si>
-    <t xml:space="preserve">Electro  Black full Sleeves Jersey with Neon Matching </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Orange Full Sleeves Jersey with Navy Blue Matching </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro Black Full Sleeves Jersey With Neon Matching </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Dark Sky Blue Colour Jersey </t>
   </si>
   <si>
-    <t xml:space="preserve">Electro Light Blue Full Sleeves with Sublimation Sleeves Made of Nirmal Net Fabric </t>
-  </si>
-  <si>
     <t>Electro Grey Full Sleeves with Red and White Patch</t>
   </si>
   <si>
-    <t xml:space="preserve">Electro Neon Pink Full Sleeves  Jersey with matching Royal Blue  Made of Nirmal Net Fabric </t>
-  </si>
-  <si>
-    <t>Electro Orange Full Sleeves Jersey with White &amp; Black Matching Made of Nirmal Net Fabric</t>
-  </si>
-  <si>
-    <t>Electro Dry-fit full sleeves Jersey Black &amp; Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electro Dry-fit full sleeves Jersey Black &amp; Neon Matching </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electro Dry-fit full sleeves Jersey white with matching Royal Blue </t>
   </si>
   <si>
@@ -1958,24 +1901,12 @@
     <t xml:space="preserve">Electro Two Stripes Jersey Made of Netted Fabric </t>
   </si>
   <si>
-    <t>Electro Rangler  Jersey  Matching Black with Grey</t>
-  </si>
-  <si>
-    <t>Electro Rangler Jersey Matching Navy Blue with Yellow</t>
-  </si>
-  <si>
     <t>Electro yellow full sleeves  Jersey with Matching Pattern</t>
   </si>
   <si>
-    <t>Electro Navy Blue Full Sleeves Jersey with Neon Matching Pattern</t>
-  </si>
-  <si>
     <t>Electro white full sleeves Jersey with Matching Patternwith Three Strips</t>
   </si>
   <si>
-    <t xml:space="preserve">Electro Yellow Full Sleeves with Red &amp; black matching PatternMade of Nirnal Net Fabric </t>
-  </si>
-  <si>
     <t>Electro Black Full Sleeves Jersey With Matching Pattern</t>
   </si>
   <si>
@@ -1986,21 +1917,6 @@
   </si>
   <si>
     <t xml:space="preserve">Electro Digital Print Sublimation T-shirt </t>
-  </si>
-  <si>
-    <t>Electro Rangler Jersey matching Navy Blue with White</t>
-  </si>
-  <si>
-    <t>Electro Rangler Jersey matching Navy Blue with Orange</t>
-  </si>
-  <si>
-    <t>Electro Rangler Jersey matching Royal Blue with Yellow</t>
-  </si>
-  <si>
-    <t>Electro Rangler Jersey matching Orange with Navy Blue</t>
-  </si>
-  <si>
-    <t>Electro Rangler Jersey matching Yellow with Royal Blue</t>
   </si>
   <si>
     <t>Electro V-Cum Colar Melange T-shirts</t>
@@ -2046,63 +1962,267 @@
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Electro Pink with Sublimation Patch Jersey</t>
-  </si>
-  <si>
-    <t>Get this Black Colour With Neon Pattern Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+    <t>Electro Black With (Neon Pattern) Jersey</t>
+  </si>
+  <si>
+    <t>Electro Pink with (Sublimation Patch) Jersey</t>
+  </si>
+  <si>
+    <t>Electro Tri Colour Jersey With (Sublimation Print)</t>
+  </si>
+  <si>
+    <t>Electro Navy blue  With (Neon Pattern Jersey)</t>
+  </si>
+  <si>
+    <t>Electro white with (Light Blue Matching Jersey )</t>
+  </si>
+  <si>
+    <t>Electro Royal Blue with (white &amp; Black Matching )</t>
+  </si>
+  <si>
+    <t>Electro white white matching (Orange and Blue Jersey )</t>
+  </si>
+  <si>
+    <t>Electro Black Jersey with (sublimation Patch)</t>
+  </si>
+  <si>
+    <t>Electro White with matching (Pink &amp; Black Jersey )</t>
+  </si>
+  <si>
+    <t>Electro Navy Blue Jersey Matching (red &amp; white)</t>
+  </si>
+  <si>
+    <t>Electro Black Jersey with matching (Red &amp; grey)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro  Black full Sleeves Jersey with ( Neon Matching ) </t>
+  </si>
+  <si>
+    <t>Electro Navy Blue Full Sleeves Jersey with ( Neon Matching ) Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Black Full Sleeves Jersey With ( Neon Matching ) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electro Dry-fit full sleeves Jersey Black &amp; ( Neon Matching ) </t>
+  </si>
+  <si>
+    <t>Electro Rangler  Jersey  Matching (Black with Grey)</t>
+  </si>
+  <si>
+    <t>Electro Rangler Jersey Matching (Navy Blue with Yellow)</t>
+  </si>
+  <si>
+    <t>Electro Rangler Jersey matching (Navy Blue with White)</t>
+  </si>
+  <si>
+    <t>Electro Rangler Jersey matching (Navy Blue with Orange)</t>
+  </si>
+  <si>
+    <t>Electro Rangler Jersey matching (Royal Blue with Yellow)</t>
+  </si>
+  <si>
+    <t>Electro Rangler Jersey matching (Orange with Navy Blue)</t>
+  </si>
+  <si>
+    <t>Electro Rangler Jersey matching (Yellow with Royal Blue)</t>
+  </si>
+  <si>
+    <t>Electro Black Jersey with ( Neon Matching )</t>
+  </si>
+  <si>
+    <t>Electro Yellow Full Sleeves with Red &amp; black matching Pattern</t>
+  </si>
+  <si>
+    <t>Electro Light Blue Full Sleeves with Sublimation Sleeves</t>
+  </si>
+  <si>
+    <t>Electro Neon Pink Full Sleeves  Jersey with matching Royal Blue</t>
+  </si>
+  <si>
+    <t>Electro Orange Full Sleeves Jersey with White &amp; Black Matching</t>
+  </si>
+  <si>
+    <t>Electro Dry-fit full sleeves Jersey (Black &amp; Red)</t>
+  </si>
+  <si>
+    <t>Electro Sky blue Jersey with macthing Patches</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
 Fabric          : Polyester(100%)
 Sleeve        : Short Hand Sleeve
 Neck            : Colar Neck 
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Yellow with Mix Colour patch Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester
+Sleeve        : Full Sleeves
+Neck            : Round V-neck
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester
+Sleeve        : Full Sleeves
+Neck            : Collar
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester
+Sleeve        : Full Sleeves
+Neck            : V-Neck Collar
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester
+Sleeve        : Short Hand Sleeves
+Neck            : Collar
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester (100%)
+Sleeve        : Short Hand Sleeves
+Neck            : V-Neck Collar
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester (100%)
+Sleeve        : Short Hand Sleeves
+Neck            : Round Neck
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light PC Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor For Advertising ,Branding ,Promotion Activity in MNC.
+Fabric          : Polyester (50%) Cotton (50%)
+Sleeve        : Short Hand Sleeves
+Neck            : Collar
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light PC Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor wear
+Fabric          : Lycra (4 Way)
+Sleeve        : Full Hand Sleeve
+Neck            : Round Neck 
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Nirmal Net (NETTED) Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Nirmal Netted
 Sleeve        : Short Hand Sleeve
 Neck            : Colar Neck 
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Royal Blue Colour  Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Dry-Fit Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Dry - Fit
 Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
+Neck            : Crew Neck
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Tri Colour  Jersey with Sublimation Print from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester ( Sublimation Print On Front Side )
+Sleeve        : Full Hand Sleeve
+Neck            : Collar
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polyester ( Sublimation Print On Front Side )
 Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
+Neck            : Collar
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Navy Blue Colour  Jersey with Neon Matching from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
-Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Netted Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Nirmal Net ( NETTED )
+Sleeve        : Full Sleeves
+Neck            : Collar
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Black Colour  Jersey with Neon Matching from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
-Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Dry-Fit Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Dry-Fit
+Sleeve        : Full Sleeves
+Neck            : Round V-neck
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Yellow Colour jersey with Matching Pattern from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
-Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Nirmal Net (NETTED) Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Nirmal Net ( NETTED )
+Sleeve        : Short Hand  Sleeves
+Neck            : Collar
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
   </si>
   <si>
-    <t>Get this Navy Blue Colour jersey with Red &amp;Grey Matching from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Light Polyester Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
-Fabric          : Polyester(100%)
-Sleeve        : Short Hand Sleeve
-Neck            : Colar Neck 
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Polymelange Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Polymelange
+Sleeve        : Short Hand Sleeves
+Neck            : V-Neck Collar
 Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Netted (Dot Net / Rice Net) Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor sports activities like Cricket, Running, Walking, Jogging, Yoga, Golf, Aerobics, Hockey, Fitness, Gym, Water sports, Swimming, Football, Surfing, Volleyball etc
+Fabric          : Netted (Dot Net / Rice Net)
+Sleeve        : Short Hand Sleeves
+Neck            : Crew Round Neck 
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Get this Impressive Jersey from Electro.Electro  Proudly Presents This Tshirt Made Out Of The Super Poly  Fabric. This Fabric Transports Moisture Away From The Body, Keeping You Cool And Dry. Quick Dry Out and moisture management of the fabric offers coolness &amp; dryness even in during highest level of sweat.This T shirt is ideal for all kinds of indoor and outdoor wear
+Fabric          : Superpoly
+Sleeve        : Full Hand Sleeve
+Neck            : Collar
+Zip                : Yes 
+Note : Now You Can Customize This T-shirt As Per Your Requirement</t>
+  </si>
+  <si>
+    <t>Polyester</t>
+  </si>
+  <si>
+    <t>DRY-FIT</t>
+  </si>
+  <si>
+    <t>Nirmal Net</t>
+  </si>
+  <si>
+    <t>Dry-fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nirmal Net </t>
+  </si>
+  <si>
+    <t>Polmelange</t>
+  </si>
+  <si>
+    <t>Rice Net / Dot Net</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Lycra</t>
+  </si>
+  <si>
+    <t>Superpoly</t>
+  </si>
+  <si>
+    <t>All Size S  M  L  XL  2XL</t>
+  </si>
+  <si>
+    <t>Pack of 3 in One Pack</t>
+  </si>
+  <si>
+    <t>32  36  40  42  44  46  48</t>
+  </si>
+  <si>
+    <t>33  36  40  42  44  46  48</t>
   </si>
 </sst>
 </file>
@@ -2247,7 +2367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2303,6 +2423,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2601,7 +2725,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="H161" sqref="H161:H162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2609,10 +2733,11 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="83.7109375" customWidth="1"/>
-    <col min="5" max="5" width="68.140625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2658,7 +2783,16 @@
         <v>597</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>662</v>
+        <v>634</v>
+      </c>
+      <c r="F2">
+        <v>142</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2672,10 +2806,19 @@
         <v>485</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>598</v>
+        <v>635</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>664</v>
+      </c>
+      <c r="F3">
+        <v>142</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2689,10 +2832,19 @@
         <v>486</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>663</v>
+        <v>636</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>664</v>
+      </c>
+      <c r="F4">
+        <v>142</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2706,10 +2858,19 @@
         <v>487</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>665</v>
+        <v>664</v>
+      </c>
+      <c r="F5">
+        <v>142</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2723,10 +2884,19 @@
         <v>488</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>666</v>
+        <v>664</v>
+      </c>
+      <c r="F6">
+        <v>142</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2740,10 +2910,19 @@
         <v>489</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>601</v>
+        <v>637</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>667</v>
+        <v>664</v>
+      </c>
+      <c r="F7">
+        <v>132</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2757,10 +2936,19 @@
         <v>490</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>602</v>
+        <v>638</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>668</v>
+        <v>664</v>
+      </c>
+      <c r="F8">
+        <v>142</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2774,10 +2962,19 @@
         <v>491</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>603</v>
+        <v>657</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>669</v>
+        <v>664</v>
+      </c>
+      <c r="F9">
+        <v>142</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2791,6 +2988,18 @@
         <v>492</v>
       </c>
       <c r="D10" s="13"/>
+      <c r="E10" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F10">
+        <v>142</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
@@ -2803,10 +3012,19 @@
         <v>493</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>670</v>
+        <v>664</v>
+      </c>
+      <c r="F11">
+        <v>142</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -2820,10 +3038,19 @@
         <v>494</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>643</v>
+        <v>620</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
+      </c>
+      <c r="F12">
+        <v>142</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -2837,7 +3064,19 @@
         <v>495</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>605</v>
+        <v>639</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F13">
+        <v>142</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2851,7 +3090,19 @@
         <v>496</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>606</v>
+        <v>601</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F14">
+        <v>142</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2865,7 +3116,19 @@
         <v>497</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>607</v>
+        <v>640</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F15">
+        <v>142</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2879,7 +3142,19 @@
         <v>498</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>608</v>
+        <v>602</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F16">
+        <v>142</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2893,7 +3168,19 @@
         <v>499</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>624</v>
+        <v>610</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F17">
+        <v>142</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -2907,7 +3194,19 @@
         <v>500</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>609</v>
+        <v>603</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F18">
+        <v>142</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2921,7 +3220,19 @@
         <v>501</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>610</v>
+        <v>641</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F19">
+        <v>142</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2935,7 +3246,19 @@
         <v>502</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>611</v>
+        <v>663</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F20">
+        <v>142</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2949,7 +3272,19 @@
         <v>503</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>612</v>
+        <v>642</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="F21">
+        <v>152</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="8" customFormat="1">
@@ -2974,7 +3309,19 @@
         <v>510</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>613</v>
+        <v>604</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="F23">
+        <v>154</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2988,7 +3335,19 @@
         <v>511</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>614</v>
+        <v>643</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="F24">
+        <v>175</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -3002,7 +3361,19 @@
         <v>512</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>615</v>
+        <v>644</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="F25">
+        <v>175</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -3016,7 +3387,19 @@
         <v>513</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>618</v>
+        <v>606</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="F26">
+        <v>175</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -3030,7 +3413,19 @@
         <v>514</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>616</v>
+        <v>605</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="F27">
+        <v>175</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -3044,7 +3439,19 @@
         <v>515</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>617</v>
+        <v>645</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>673</v>
+      </c>
+      <c r="F28">
+        <v>175</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="8" customFormat="1">
@@ -3069,7 +3476,19 @@
         <v>516</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>619</v>
+        <v>607</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="F30">
+        <v>165</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>684</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3083,7 +3502,19 @@
         <v>517</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>620</v>
+        <v>608</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>674</v>
+      </c>
+      <c r="F31">
+        <v>170</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>684</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1">
@@ -3108,7 +3539,19 @@
         <v>518</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>621</v>
+        <v>646</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="F33">
+        <v>165</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -3122,7 +3565,19 @@
         <v>519</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>637</v>
+        <v>616</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="F34">
+        <v>165</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -3136,7 +3591,19 @@
         <v>520</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>638</v>
+        <v>647</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="F35">
+        <v>165</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -3150,7 +3617,19 @@
         <v>521</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>639</v>
+        <v>617</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="F36">
+        <v>165</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3164,7 +3643,19 @@
         <v>522</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>622</v>
+        <v>609</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="F37">
+        <v>165</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3178,7 +3669,19 @@
         <v>523</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>623</v>
+        <v>648</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="F38">
+        <v>165</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1">
@@ -3203,7 +3706,19 @@
         <v>524</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>640</v>
+        <v>658</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F40">
+        <v>184</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3217,7 +3732,19 @@
         <v>525</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>625</v>
+        <v>659</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F41">
+        <v>207</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -3231,7 +3758,19 @@
         <v>526</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>626</v>
+        <v>611</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F42">
+        <v>194</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3245,7 +3784,19 @@
         <v>527</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>627</v>
+        <v>660</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F43">
+        <v>194</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3259,7 +3810,19 @@
         <v>528</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>641</v>
+        <v>618</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F44">
+        <v>194</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -3273,7 +3836,19 @@
         <v>529</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>642</v>
+        <v>619</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F45">
+        <v>194</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3287,7 +3862,19 @@
         <v>530</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>628</v>
+        <v>661</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>677</v>
+      </c>
+      <c r="F46">
+        <v>194</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1">
@@ -3312,7 +3899,19 @@
         <v>531</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>629</v>
+        <v>662</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="F48">
+        <v>180</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3326,7 +3925,19 @@
         <v>532</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>630</v>
+        <v>649</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="F49">
+        <v>180</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3340,7 +3951,19 @@
         <v>533</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>631</v>
+        <v>612</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="F50">
+        <v>180</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3354,7 +3977,19 @@
         <v>534</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>632</v>
+        <v>613</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>678</v>
+      </c>
+      <c r="F51">
+        <v>207</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="8" customFormat="1">
@@ -3379,7 +4014,19 @@
         <v>535</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F53">
+        <v>181</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3393,7 +4040,19 @@
         <v>536</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F54">
+        <v>181</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3407,7 +4066,19 @@
         <v>537</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F55">
+        <v>181</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3421,7 +4092,19 @@
         <v>538</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F56">
+        <v>181</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3435,7 +4118,19 @@
         <v>539</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F57">
+        <v>181</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -3449,7 +4144,19 @@
         <v>540</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F58">
+        <v>181</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3463,7 +4170,19 @@
         <v>541</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F59">
+        <v>181</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3477,7 +4196,19 @@
         <v>542</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F60">
+        <v>181</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3491,7 +4222,19 @@
         <v>543</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F61">
+        <v>181</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3505,7 +4248,19 @@
         <v>544</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>633</v>
+        <v>614</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>675</v>
+      </c>
+      <c r="F62">
+        <v>181</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3519,7 +4274,19 @@
         <v>545</v>
       </c>
       <c r="D63" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F63">
+        <v>162</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3533,10 +4300,22 @@
         <v>546</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F64">
+        <v>162</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="2" t="s">
         <v>57</v>
       </c>
@@ -3547,10 +4326,22 @@
         <v>547</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F65">
+        <v>162</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="2" t="s">
         <v>58</v>
       </c>
@@ -3561,10 +4352,22 @@
         <v>548</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F66">
+        <v>162</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="2" t="s">
         <v>59</v>
       </c>
@@ -3575,10 +4378,22 @@
         <v>549</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F67">
+        <v>162</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="2" t="s">
         <v>60</v>
       </c>
@@ -3589,10 +4404,22 @@
         <v>550</v>
       </c>
       <c r="D68" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F68">
+        <v>162</v>
+      </c>
+      <c r="G68" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H68" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="2" t="s">
         <v>61</v>
       </c>
@@ -3603,10 +4430,22 @@
         <v>551</v>
       </c>
       <c r="D69" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F69">
+        <v>162</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H69" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="2" t="s">
         <v>62</v>
       </c>
@@ -3617,10 +4456,22 @@
         <v>552</v>
       </c>
       <c r="D70" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F70">
+        <v>162</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="2" t="s">
         <v>63</v>
       </c>
@@ -3631,10 +4482,22 @@
         <v>553</v>
       </c>
       <c r="D71" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F71">
+        <v>162</v>
+      </c>
+      <c r="G71" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="2" t="s">
         <v>64</v>
       </c>
@@ -3645,10 +4508,22 @@
         <v>554</v>
       </c>
       <c r="D72" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F72">
+        <v>162</v>
+      </c>
+      <c r="G72" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="2" t="s">
         <v>65</v>
       </c>
@@ -3659,10 +4534,22 @@
         <v>555</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F73">
+        <v>162</v>
+      </c>
+      <c r="G73" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="2" t="s">
         <v>66</v>
       </c>
@@ -3673,10 +4560,22 @@
         <v>556</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F74">
+        <v>162</v>
+      </c>
+      <c r="G74" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="2" t="s">
         <v>67</v>
       </c>
@@ -3687,10 +4586,22 @@
         <v>557</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F75">
+        <v>162</v>
+      </c>
+      <c r="G75" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="2" t="s">
         <v>68</v>
       </c>
@@ -3701,10 +4612,22 @@
         <v>558</v>
       </c>
       <c r="D76" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F76">
+        <v>162</v>
+      </c>
+      <c r="G76" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="2" t="s">
         <v>69</v>
       </c>
@@ -3715,10 +4638,22 @@
         <v>559</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F77">
+        <v>162</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
@@ -3729,10 +4664,22 @@
         <v>560</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F78">
+        <v>162</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="2" t="s">
         <v>71</v>
       </c>
@@ -3743,10 +4690,22 @@
         <v>561</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>621</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F79">
+        <v>162</v>
+      </c>
+      <c r="G79" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="2" t="s">
         <v>72</v>
       </c>
@@ -3757,7 +4716,19 @@
         <v>562</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F80">
+        <v>162</v>
+      </c>
+      <c r="G80" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -3771,7 +4742,19 @@
         <v>563</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F81">
+        <v>162</v>
+      </c>
+      <c r="G81" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="82" spans="1:9">
@@ -3785,7 +4768,19 @@
         <v>564</v>
       </c>
       <c r="D82" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F82">
+        <v>162</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="83" spans="1:9">
@@ -3799,7 +4794,19 @@
         <v>565</v>
       </c>
       <c r="D83" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F83">
+        <v>162</v>
+      </c>
+      <c r="G83" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="84" spans="1:9">
@@ -3813,7 +4820,19 @@
         <v>566</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F84">
+        <v>162</v>
+      </c>
+      <c r="G84" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="85" spans="1:9">
@@ -3827,7 +4846,19 @@
         <v>567</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F85">
+        <v>162</v>
+      </c>
+      <c r="G85" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="86" spans="1:9">
@@ -3841,7 +4872,19 @@
         <v>568</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F86">
+        <v>162</v>
+      </c>
+      <c r="G86" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="87" spans="1:9">
@@ -3855,7 +4898,19 @@
         <v>569</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>644</v>
+        <v>621</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="F87">
+        <v>162</v>
+      </c>
+      <c r="G87" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="8" customFormat="1">
@@ -3880,6 +4935,18 @@
         <v>447</v>
       </c>
       <c r="D89" s="16"/>
+      <c r="E89" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F89">
+        <v>129</v>
+      </c>
+      <c r="G89" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="2" t="s">
@@ -3892,7 +4959,19 @@
         <v>570</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F90">
+        <v>129</v>
+      </c>
+      <c r="G90" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H90" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="91" spans="1:9">
@@ -3906,7 +4985,19 @@
         <v>571</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F91" s="8">
+        <v>129</v>
+      </c>
+      <c r="G91" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="92" spans="1:9">
@@ -3920,7 +5011,19 @@
         <v>572</v>
       </c>
       <c r="D92" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F92" s="8">
+        <v>129</v>
+      </c>
+      <c r="G92" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H92" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -3934,7 +5037,19 @@
         <v>573</v>
       </c>
       <c r="D93" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F93" s="8">
+        <v>129</v>
+      </c>
+      <c r="G93" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="94" spans="1:9">
@@ -3948,7 +5063,19 @@
         <v>574</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F94" s="8">
+        <v>129</v>
+      </c>
+      <c r="G94" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H94" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -3962,7 +5089,19 @@
         <v>575</v>
       </c>
       <c r="D95" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F95" s="8">
+        <v>129</v>
+      </c>
+      <c r="G95" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H95" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="96" spans="1:9">
@@ -3976,7 +5115,19 @@
         <v>576</v>
       </c>
       <c r="D96" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F96" s="8">
+        <v>129</v>
+      </c>
+      <c r="G96" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H96" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="97" spans="1:9">
@@ -3990,7 +5141,19 @@
         <v>577</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F97" s="8">
+        <v>129</v>
+      </c>
+      <c r="G97" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H97" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="98" spans="1:9">
@@ -4004,7 +5167,19 @@
         <v>578</v>
       </c>
       <c r="D98" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F98" s="8">
+        <v>129</v>
+      </c>
+      <c r="G98" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H98" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="99" spans="1:9">
@@ -4018,7 +5193,19 @@
         <v>579</v>
       </c>
       <c r="D99" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F99" s="8">
+        <v>129</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H99" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="100" spans="1:9">
@@ -4032,7 +5219,19 @@
         <v>580</v>
       </c>
       <c r="D100" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F100" s="8">
+        <v>129</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H100" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="101" spans="1:9">
@@ -4046,7 +5245,19 @@
         <v>581</v>
       </c>
       <c r="D101" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F101" s="8">
+        <v>129</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H101" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="102" spans="1:9">
@@ -4060,7 +5271,19 @@
         <v>582</v>
       </c>
       <c r="D102" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F102" s="8">
+        <v>129</v>
+      </c>
+      <c r="G102" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H102" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="103" spans="1:9">
@@ -4074,7 +5297,19 @@
         <v>583</v>
       </c>
       <c r="D103" s="12" t="s">
-        <v>634</v>
+        <v>615</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>679</v>
+      </c>
+      <c r="F103" s="8">
+        <v>139</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="H103" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="104" spans="1:9" s="8" customFormat="1">
@@ -4099,7 +5334,19 @@
         <v>584</v>
       </c>
       <c r="D105" s="12" t="s">
-        <v>635</v>
+        <v>650</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F105">
+        <v>111</v>
+      </c>
+      <c r="G105" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H105" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="106" spans="1:9">
@@ -4113,7 +5360,19 @@
         <v>586</v>
       </c>
       <c r="D106" s="12" t="s">
-        <v>636</v>
+        <v>651</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F106">
+        <v>111</v>
+      </c>
+      <c r="G106" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H106" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="107" spans="1:9">
@@ -4127,7 +5386,19 @@
         <v>585</v>
       </c>
       <c r="D107" s="12" t="s">
-        <v>645</v>
+        <v>652</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F107">
+        <v>111</v>
+      </c>
+      <c r="G107" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H107" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="108" spans="1:9">
@@ -4141,7 +5412,19 @@
         <v>587</v>
       </c>
       <c r="D108" s="12" t="s">
-        <v>646</v>
+        <v>653</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F108">
+        <v>111</v>
+      </c>
+      <c r="G108" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H108" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -4155,7 +5438,19 @@
         <v>588</v>
       </c>
       <c r="D109" s="12" t="s">
-        <v>647</v>
+        <v>654</v>
+      </c>
+      <c r="E109" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F109">
+        <v>111</v>
+      </c>
+      <c r="G109" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H109" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="110" spans="1:9">
@@ -4169,7 +5464,19 @@
         <v>589</v>
       </c>
       <c r="D110" s="12" t="s">
-        <v>648</v>
+        <v>655</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F110">
+        <v>111</v>
+      </c>
+      <c r="G110" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H110" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -4183,7 +5490,19 @@
         <v>590</v>
       </c>
       <c r="D111" s="12" t="s">
-        <v>649</v>
+        <v>656</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>668</v>
+      </c>
+      <c r="F111">
+        <v>111</v>
+      </c>
+      <c r="G111" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H111" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="112" spans="1:9" s="8" customFormat="1">
@@ -4208,7 +5527,19 @@
         <v>591</v>
       </c>
       <c r="D113" s="12" t="s">
-        <v>650</v>
+        <v>622</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="F113">
+        <v>131</v>
+      </c>
+      <c r="G113" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="H113" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="114" spans="1:9">
@@ -4222,7 +5553,19 @@
         <v>592</v>
       </c>
       <c r="D114" s="12" t="s">
-        <v>650</v>
+        <v>622</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="F114" s="8">
+        <v>131</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="H114" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="115" spans="1:9">
@@ -4236,7 +5579,19 @@
         <v>593</v>
       </c>
       <c r="D115" s="12" t="s">
-        <v>650</v>
+        <v>622</v>
+      </c>
+      <c r="E115" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="F115" s="8">
+        <v>131</v>
+      </c>
+      <c r="G115" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="H115" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="116" spans="1:9">
@@ -4250,7 +5605,19 @@
         <v>594</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>650</v>
+        <v>622</v>
+      </c>
+      <c r="E116" s="10" t="s">
+        <v>680</v>
+      </c>
+      <c r="F116" s="8">
+        <v>131</v>
+      </c>
+      <c r="G116" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="H116" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="8" customFormat="1">
@@ -4275,7 +5642,19 @@
         <v>595</v>
       </c>
       <c r="D118" s="12" t="s">
-        <v>650</v>
+        <v>622</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="F118" s="22">
+        <v>99</v>
+      </c>
+      <c r="G118" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H118" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -4289,7 +5668,19 @@
         <v>596</v>
       </c>
       <c r="D119" s="12" t="s">
-        <v>650</v>
+        <v>622</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>669</v>
+      </c>
+      <c r="F119" s="22">
+        <v>99</v>
+      </c>
+      <c r="G119" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H119" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="8" customFormat="1">
@@ -4314,7 +5705,19 @@
         <v>448</v>
       </c>
       <c r="D121" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F121">
+        <v>117</v>
+      </c>
+      <c r="G121" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H121" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -4328,7 +5731,19 @@
         <v>449</v>
       </c>
       <c r="D122" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E122" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F122">
+        <v>117</v>
+      </c>
+      <c r="G122" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H122" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="123" spans="1:9">
@@ -4342,7 +5757,19 @@
         <v>450</v>
       </c>
       <c r="D123" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F123">
+        <v>117</v>
+      </c>
+      <c r="G123" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H123" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -4356,7 +5783,19 @@
         <v>451</v>
       </c>
       <c r="D124" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F124">
+        <v>117</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H124" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="125" spans="1:9">
@@ -4370,7 +5809,19 @@
         <v>452</v>
       </c>
       <c r="D125" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F125">
+        <v>117</v>
+      </c>
+      <c r="G125" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H125" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="126" spans="1:9">
@@ -4384,7 +5835,19 @@
         <v>453</v>
       </c>
       <c r="D126" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F126">
+        <v>117</v>
+      </c>
+      <c r="G126" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H126" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="127" spans="1:9">
@@ -4398,7 +5861,19 @@
         <v>454</v>
       </c>
       <c r="D127" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F127">
+        <v>117</v>
+      </c>
+      <c r="G127" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H127" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="128" spans="1:9">
@@ -4412,7 +5887,19 @@
         <v>455</v>
       </c>
       <c r="D128" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E128" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F128">
+        <v>117</v>
+      </c>
+      <c r="G128" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H128" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="129" spans="1:9">
@@ -4426,7 +5913,19 @@
         <v>456</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E129" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F129">
+        <v>117</v>
+      </c>
+      <c r="G129" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H129" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -4440,7 +5939,19 @@
         <v>457</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E130" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F130">
+        <v>117</v>
+      </c>
+      <c r="G130" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H130" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="131" spans="1:9">
@@ -4454,7 +5965,19 @@
         <v>458</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E131" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F131">
+        <v>117</v>
+      </c>
+      <c r="G131" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H131" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -4468,7 +5991,19 @@
         <v>459</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E132" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F132">
+        <v>117</v>
+      </c>
+      <c r="G132" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H132" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="133" spans="1:9">
@@ -4482,7 +6017,19 @@
         <v>460</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>651</v>
+        <v>623</v>
+      </c>
+      <c r="E133" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F133">
+        <v>117</v>
+      </c>
+      <c r="G133" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H133" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="134" spans="1:9">
@@ -4496,7 +6043,19 @@
         <v>461</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>652</v>
+        <v>624</v>
+      </c>
+      <c r="E134" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F134">
+        <v>95</v>
+      </c>
+      <c r="G134" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H134" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="135" spans="1:9">
@@ -4510,7 +6069,19 @@
         <v>462</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>652</v>
+        <v>624</v>
+      </c>
+      <c r="E135" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F135">
+        <v>95</v>
+      </c>
+      <c r="G135" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H135" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="136" spans="1:9">
@@ -4524,7 +6095,19 @@
         <v>463</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>652</v>
+        <v>624</v>
+      </c>
+      <c r="E136" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F136">
+        <v>95</v>
+      </c>
+      <c r="G136" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H136" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="137" spans="1:9">
@@ -4538,7 +6121,19 @@
         <v>464</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>652</v>
+        <v>624</v>
+      </c>
+      <c r="E137" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F137">
+        <v>95</v>
+      </c>
+      <c r="G137" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H137" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="138" spans="1:9">
@@ -4552,7 +6147,19 @@
         <v>465</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>652</v>
+        <v>624</v>
+      </c>
+      <c r="E138" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F138">
+        <v>95</v>
+      </c>
+      <c r="G138" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H138" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="139" spans="1:9">
@@ -4566,7 +6173,19 @@
         <v>466</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>652</v>
+        <v>624</v>
+      </c>
+      <c r="E139" s="10" t="s">
+        <v>681</v>
+      </c>
+      <c r="F139">
+        <v>95</v>
+      </c>
+      <c r="G139" s="12" t="s">
+        <v>689</v>
+      </c>
+      <c r="H139" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="140" spans="1:9" s="8" customFormat="1">
@@ -4591,7 +6210,19 @@
         <v>467</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>653</v>
+        <v>625</v>
+      </c>
+      <c r="E141" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F141">
+        <v>84</v>
+      </c>
+      <c r="G141" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H141" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="142" spans="1:9">
@@ -4605,7 +6236,19 @@
         <v>468</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>654</v>
+        <v>626</v>
+      </c>
+      <c r="E142" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F142">
+        <v>84</v>
+      </c>
+      <c r="G142" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H142" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="143" spans="1:9">
@@ -4619,7 +6262,19 @@
         <v>469</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>655</v>
+        <v>627</v>
+      </c>
+      <c r="E143" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F143">
+        <v>84</v>
+      </c>
+      <c r="G143" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H143" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="144" spans="1:9">
@@ -4633,7 +6288,19 @@
         <v>470</v>
       </c>
       <c r="D144" s="12" t="s">
-        <v>656</v>
+        <v>628</v>
+      </c>
+      <c r="E144" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F144">
+        <v>84</v>
+      </c>
+      <c r="G144" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H144" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="145" spans="1:9">
@@ -4647,7 +6314,19 @@
         <v>471</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>657</v>
+        <v>629</v>
+      </c>
+      <c r="E145" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F145">
+        <v>84</v>
+      </c>
+      <c r="G145" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H145" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="146" spans="1:9">
@@ -4661,7 +6340,19 @@
         <v>472</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>658</v>
+        <v>630</v>
+      </c>
+      <c r="E146" s="10" t="s">
+        <v>670</v>
+      </c>
+      <c r="F146">
+        <v>84</v>
+      </c>
+      <c r="G146" s="13" t="s">
+        <v>683</v>
+      </c>
+      <c r="H146" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="147" spans="1:9" s="8" customFormat="1">
@@ -4686,7 +6377,19 @@
         <v>473</v>
       </c>
       <c r="D148" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E148" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F148">
+        <v>150</v>
+      </c>
+      <c r="G148" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H148" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="149" spans="1:9">
@@ -4700,7 +6403,19 @@
         <v>474</v>
       </c>
       <c r="D149" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E149" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F149">
+        <v>150</v>
+      </c>
+      <c r="G149" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H149" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="150" spans="1:9">
@@ -4714,7 +6429,19 @@
         <v>475</v>
       </c>
       <c r="D150" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E150" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F150">
+        <v>150</v>
+      </c>
+      <c r="G150" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H150" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="151" spans="1:9">
@@ -4728,7 +6455,19 @@
         <v>476</v>
       </c>
       <c r="D151" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E151" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F151">
+        <v>150</v>
+      </c>
+      <c r="G151" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H151" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="152" spans="1:9">
@@ -4742,7 +6481,19 @@
         <v>477</v>
       </c>
       <c r="D152" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E152" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F152">
+        <v>150</v>
+      </c>
+      <c r="G152" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H152" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="153" spans="1:9">
@@ -4756,7 +6507,19 @@
         <v>478</v>
       </c>
       <c r="D153" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E153" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F153">
+        <v>150</v>
+      </c>
+      <c r="G153" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H153" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="154" spans="1:9">
@@ -4770,7 +6533,19 @@
         <v>479</v>
       </c>
       <c r="D154" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E154" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F154">
+        <v>150</v>
+      </c>
+      <c r="G154" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H154" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="155" spans="1:9">
@@ -4784,7 +6559,19 @@
         <v>480</v>
       </c>
       <c r="D155" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E155" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F155">
+        <v>150</v>
+      </c>
+      <c r="G155" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H155" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="156" spans="1:9">
@@ -4798,7 +6585,19 @@
         <v>481</v>
       </c>
       <c r="D156" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E156" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F156">
+        <v>150</v>
+      </c>
+      <c r="G156" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H156" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="157" spans="1:9">
@@ -4812,7 +6611,19 @@
         <v>482</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>659</v>
+        <v>631</v>
+      </c>
+      <c r="E157" s="10" t="s">
+        <v>671</v>
+      </c>
+      <c r="F157">
+        <v>150</v>
+      </c>
+      <c r="G157" s="12" t="s">
+        <v>690</v>
+      </c>
+      <c r="H157" s="13" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="158" spans="1:9" s="8" customFormat="1">
@@ -4837,7 +6648,19 @@
         <v>483</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>660</v>
+        <v>632</v>
+      </c>
+      <c r="E159" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="F159">
+        <v>209</v>
+      </c>
+      <c r="G159" s="12" t="s">
+        <v>691</v>
+      </c>
+      <c r="H159" s="12" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="160" spans="1:9">
@@ -4851,7 +6674,19 @@
         <v>484</v>
       </c>
       <c r="D160" s="11" t="s">
-        <v>660</v>
+        <v>632</v>
+      </c>
+      <c r="E160" s="10" t="s">
+        <v>672</v>
+      </c>
+      <c r="F160">
+        <v>209</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>691</v>
+      </c>
+      <c r="H160" s="12" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15" customHeight="1">
@@ -4865,7 +6700,19 @@
         <v>506</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>661</v>
+        <v>633</v>
+      </c>
+      <c r="E161" s="21" t="s">
+        <v>682</v>
+      </c>
+      <c r="F161" s="8">
+        <v>475</v>
+      </c>
+      <c r="G161" s="12" t="s">
+        <v>692</v>
+      </c>
+      <c r="H161" s="12" t="s">
+        <v>695</v>
       </c>
     </row>
     <row r="162" spans="1:9">
@@ -4879,7 +6726,19 @@
         <v>509</v>
       </c>
       <c r="D162" s="11" t="s">
-        <v>661</v>
+        <v>633</v>
+      </c>
+      <c r="E162" s="10" t="s">
+        <v>682</v>
+      </c>
+      <c r="F162" s="22">
+        <v>475</v>
+      </c>
+      <c r="G162" s="12" t="s">
+        <v>692</v>
+      </c>
+      <c r="H162" s="12" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="15" customHeight="1"/>

</xml_diff>

<commit_message>
SOME MORE PRODUCT ADDED
</commit_message>
<xml_diff>
--- a/electro sports catlog details 2019-2020.xlsx
+++ b/electro sports catlog details 2019-2020.xlsx
@@ -21,7 +21,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D36" authorId="0">
+    <comment ref="E36" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="698">
   <si>
     <t>JS-01</t>
   </si>
@@ -2223,6 +2223,9 @@
   </si>
   <si>
     <t>33  36  40  42  44  46  48</t>
+  </si>
+  <si>
+    <t>Electro White Jersey with (Neon Matching Patch)</t>
   </si>
 </sst>
 </file>
@@ -2723,9 +2726,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2733,9 +2736,9 @@
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="51.7109375" customWidth="1"/>
-    <col min="5" max="5" width="123" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="6" max="6" width="123" style="8" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
   </cols>
@@ -2751,13 +2754,13 @@
         <v>147</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>445</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>149</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>152</v>
@@ -2779,14 +2782,14 @@
       <c r="C2" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8">
+        <v>142</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>634</v>
-      </c>
-      <c r="F2">
-        <v>142</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>683</v>
@@ -2805,14 +2808,14 @@
       <c r="C3" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8">
+        <v>142</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>635</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F3">
-        <v>142</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>683</v>
@@ -2831,14 +2834,14 @@
       <c r="C4" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="8">
+        <v>142</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>636</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F4">
-        <v>142</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>683</v>
@@ -2857,14 +2860,14 @@
       <c r="C5" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8">
+        <v>142</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>598</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F5">
-        <v>142</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>683</v>
@@ -2883,14 +2886,14 @@
       <c r="C6" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="8">
+        <v>142</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>599</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F6">
-        <v>142</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>683</v>
@@ -2909,14 +2912,14 @@
       <c r="C7" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="8">
+        <v>132</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>637</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F7">
-        <v>132</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>683</v>
@@ -2935,14 +2938,14 @@
       <c r="C8" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="8">
+        <v>142</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>638</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F8">
-        <v>142</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>683</v>
@@ -2961,14 +2964,14 @@
       <c r="C9" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="8">
+        <v>142</v>
+      </c>
+      <c r="E9" s="13" t="s">
         <v>657</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F9">
-        <v>142</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>683</v>
@@ -2987,12 +2990,14 @@
       <c r="C10" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="D10" s="13"/>
-      <c r="E10" s="10" t="s">
+      <c r="D10" s="8">
+        <v>142</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>697</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F10">
-        <v>142</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>683</v>
@@ -3011,14 +3016,14 @@
       <c r="C11" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="8">
+        <v>142</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>600</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F11">
-        <v>142</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>683</v>
@@ -3037,14 +3042,14 @@
       <c r="C12" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="8">
+        <v>142</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>620</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F12">
-        <v>142</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>683</v>
@@ -3063,14 +3068,14 @@
       <c r="C13" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="8">
+        <v>142</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>639</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F13">
-        <v>142</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>683</v>
@@ -3089,14 +3094,14 @@
       <c r="C14" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="8">
+        <v>142</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>601</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F14">
-        <v>142</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>683</v>
@@ -3115,14 +3120,14 @@
       <c r="C15" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="8">
+        <v>142</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>640</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F15">
-        <v>142</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>683</v>
@@ -3141,14 +3146,14 @@
       <c r="C16" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="8">
+        <v>142</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>602</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F16">
-        <v>142</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>683</v>
@@ -3167,14 +3172,14 @@
       <c r="C17" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="8">
+        <v>142</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>610</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F17">
-        <v>142</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>683</v>
@@ -3193,14 +3198,14 @@
       <c r="C18" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="8">
+        <v>142</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>603</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F18">
-        <v>142</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>683</v>
@@ -3219,14 +3224,14 @@
       <c r="C19" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="8">
+        <v>142</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>641</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="F19" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F19">
-        <v>142</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>683</v>
@@ -3245,14 +3250,14 @@
       <c r="C20" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="8">
+        <v>142</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>663</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F20">
-        <v>142</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>683</v>
@@ -3271,14 +3276,14 @@
       <c r="C21" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="8">
+        <v>152</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>642</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="10" t="s">
         <v>664</v>
-      </c>
-      <c r="F21">
-        <v>152</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>683</v>
@@ -3308,14 +3313,14 @@
       <c r="C23" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="8">
+        <v>154</v>
+      </c>
+      <c r="E23" s="13" t="s">
         <v>604</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="F23" s="10" t="s">
         <v>673</v>
-      </c>
-      <c r="F23">
-        <v>154</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>685</v>
@@ -3334,14 +3339,14 @@
       <c r="C24" s="2" t="s">
         <v>511</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="8">
+        <v>175</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>643</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>673</v>
-      </c>
-      <c r="F24">
-        <v>175</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>685</v>
@@ -3360,14 +3365,14 @@
       <c r="C25" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="8">
+        <v>175</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>644</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>673</v>
-      </c>
-      <c r="F25">
-        <v>175</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>685</v>
@@ -3386,14 +3391,14 @@
       <c r="C26" s="2" t="s">
         <v>513</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="8">
+        <v>175</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>606</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>673</v>
-      </c>
-      <c r="F26">
-        <v>175</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>685</v>
@@ -3412,14 +3417,14 @@
       <c r="C27" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="8">
+        <v>175</v>
+      </c>
+      <c r="E27" s="12" t="s">
         <v>605</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="F27" s="10" t="s">
         <v>673</v>
-      </c>
-      <c r="F27">
-        <v>175</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>685</v>
@@ -3438,14 +3443,14 @@
       <c r="C28" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="8">
+        <v>175</v>
+      </c>
+      <c r="E28" s="12" t="s">
         <v>645</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>673</v>
-      </c>
-      <c r="F28">
-        <v>175</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>685</v>
@@ -3475,14 +3480,14 @@
       <c r="C30" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="8">
+        <v>165</v>
+      </c>
+      <c r="E30" s="12" t="s">
         <v>607</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="F30" s="10" t="s">
         <v>674</v>
-      </c>
-      <c r="F30">
-        <v>165</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>684</v>
@@ -3501,14 +3506,14 @@
       <c r="C31" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="8">
+        <v>170</v>
+      </c>
+      <c r="E31" s="12" t="s">
         <v>608</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="F31" s="10" t="s">
         <v>674</v>
-      </c>
-      <c r="F31">
-        <v>170</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>684</v>
@@ -3538,14 +3543,14 @@
       <c r="C33" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="8">
+        <v>165</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>646</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="F33" s="10" t="s">
         <v>665</v>
-      </c>
-      <c r="F33">
-        <v>165</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>683</v>
@@ -3564,14 +3569,14 @@
       <c r="C34" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="8">
+        <v>165</v>
+      </c>
+      <c r="E34" s="12" t="s">
         <v>616</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="F34" s="10" t="s">
         <v>665</v>
-      </c>
-      <c r="F34">
-        <v>165</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>683</v>
@@ -3590,14 +3595,14 @@
       <c r="C35" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="8">
+        <v>165</v>
+      </c>
+      <c r="E35" s="12" t="s">
         <v>647</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="F35" s="10" t="s">
         <v>665</v>
-      </c>
-      <c r="F35">
-        <v>165</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>683</v>
@@ -3616,14 +3621,14 @@
       <c r="C36" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="8">
+        <v>165</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>617</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="F36" s="10" t="s">
         <v>665</v>
-      </c>
-      <c r="F36">
-        <v>165</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>683</v>
@@ -3642,14 +3647,14 @@
       <c r="C37" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="8">
+        <v>165</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>609</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="F37" s="10" t="s">
         <v>666</v>
-      </c>
-      <c r="F37">
-        <v>165</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>683</v>
@@ -3668,14 +3673,14 @@
       <c r="C38" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="8">
+        <v>165</v>
+      </c>
+      <c r="E38" s="12" t="s">
         <v>648</v>
       </c>
-      <c r="E38" s="10" t="s">
+      <c r="F38" s="10" t="s">
         <v>667</v>
-      </c>
-      <c r="F38">
-        <v>165</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>683</v>
@@ -3705,14 +3710,14 @@
       <c r="C40" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="8">
+        <v>184</v>
+      </c>
+      <c r="E40" s="12" t="s">
         <v>658</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F40">
-        <v>184</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>685</v>
@@ -3731,14 +3736,14 @@
       <c r="C41" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="8">
+        <v>207</v>
+      </c>
+      <c r="E41" s="12" t="s">
         <v>659</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="F41" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F41">
-        <v>207</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>685</v>
@@ -3757,14 +3762,14 @@
       <c r="C42" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="8">
+        <v>194</v>
+      </c>
+      <c r="E42" s="12" t="s">
         <v>611</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="F42" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F42">
-        <v>194</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>685</v>
@@ -3783,14 +3788,14 @@
       <c r="C43" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="8">
+        <v>194</v>
+      </c>
+      <c r="E43" s="12" t="s">
         <v>660</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="F43" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F43">
-        <v>194</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>685</v>
@@ -3809,14 +3814,14 @@
       <c r="C44" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="8">
+        <v>194</v>
+      </c>
+      <c r="E44" s="12" t="s">
         <v>618</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="F44" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F44">
-        <v>194</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>685</v>
@@ -3835,14 +3840,14 @@
       <c r="C45" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="8">
+        <v>194</v>
+      </c>
+      <c r="E45" s="12" t="s">
         <v>619</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="F45" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F45">
-        <v>194</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>685</v>
@@ -3861,14 +3866,14 @@
       <c r="C46" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="8">
+        <v>194</v>
+      </c>
+      <c r="E46" s="12" t="s">
         <v>661</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="F46" s="10" t="s">
         <v>677</v>
-      </c>
-      <c r="F46">
-        <v>194</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>685</v>
@@ -3898,14 +3903,14 @@
       <c r="C48" s="2" t="s">
         <v>531</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="8">
+        <v>180</v>
+      </c>
+      <c r="E48" s="12" t="s">
         <v>662</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="F48" s="10" t="s">
         <v>678</v>
-      </c>
-      <c r="F48">
-        <v>180</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>686</v>
@@ -3924,14 +3929,14 @@
       <c r="C49" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="8">
+        <v>180</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>649</v>
       </c>
-      <c r="E49" s="10" t="s">
+      <c r="F49" s="10" t="s">
         <v>678</v>
-      </c>
-      <c r="F49">
-        <v>180</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>686</v>
@@ -3950,14 +3955,14 @@
       <c r="C50" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="8">
+        <v>180</v>
+      </c>
+      <c r="E50" s="12" t="s">
         <v>612</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="F50" s="10" t="s">
         <v>678</v>
-      </c>
-      <c r="F50">
-        <v>180</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>686</v>
@@ -3976,14 +3981,14 @@
       <c r="C51" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="8">
+        <v>207</v>
+      </c>
+      <c r="E51" s="12" t="s">
         <v>613</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="F51" s="10" t="s">
         <v>678</v>
-      </c>
-      <c r="F51">
-        <v>207</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>686</v>
@@ -4013,14 +4018,14 @@
       <c r="C53" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="8">
+        <v>181</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="F53" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F53">
-        <v>181</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>683</v>
@@ -4039,14 +4044,14 @@
       <c r="C54" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="8">
+        <v>181</v>
+      </c>
+      <c r="E54" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="F54" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F54">
-        <v>181</v>
       </c>
       <c r="G54" s="13" t="s">
         <v>683</v>
@@ -4065,14 +4070,14 @@
       <c r="C55" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D55" s="8">
+        <v>181</v>
+      </c>
+      <c r="E55" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E55" s="10" t="s">
+      <c r="F55" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F55">
-        <v>181</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>683</v>
@@ -4091,14 +4096,14 @@
       <c r="C56" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="D56" s="12" t="s">
+      <c r="D56" s="8">
+        <v>181</v>
+      </c>
+      <c r="E56" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="F56" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F56">
-        <v>181</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>683</v>
@@ -4117,14 +4122,14 @@
       <c r="C57" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D57" s="8">
+        <v>181</v>
+      </c>
+      <c r="E57" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="F57" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F57">
-        <v>181</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>683</v>
@@ -4143,14 +4148,14 @@
       <c r="C58" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="D58" s="12" t="s">
+      <c r="D58" s="8">
+        <v>181</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="F58" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F58">
-        <v>181</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>683</v>
@@ -4169,14 +4174,14 @@
       <c r="C59" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="D59" s="12" t="s">
+      <c r="D59" s="8">
+        <v>181</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="F59" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F59">
-        <v>181</v>
       </c>
       <c r="G59" s="13" t="s">
         <v>683</v>
@@ -4195,14 +4200,14 @@
       <c r="C60" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="D60" s="12" t="s">
+      <c r="D60" s="8">
+        <v>181</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="F60" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F60">
-        <v>181</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>683</v>
@@ -4221,14 +4226,14 @@
       <c r="C61" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="8">
+        <v>181</v>
+      </c>
+      <c r="E61" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E61" s="10" t="s">
+      <c r="F61" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F61">
-        <v>181</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>683</v>
@@ -4247,14 +4252,14 @@
       <c r="C62" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="D62" s="12" t="s">
+      <c r="D62" s="8">
+        <v>181</v>
+      </c>
+      <c r="E62" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="F62" s="10" t="s">
         <v>675</v>
-      </c>
-      <c r="F62">
-        <v>181</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>683</v>
@@ -4273,14 +4278,14 @@
       <c r="C63" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="D63" s="12" t="s">
+      <c r="D63" s="8">
+        <v>162</v>
+      </c>
+      <c r="E63" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="F63" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F63">
-        <v>162</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>683</v>
@@ -4299,14 +4304,14 @@
       <c r="C64" s="2" t="s">
         <v>546</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="D64" s="8">
+        <v>162</v>
+      </c>
+      <c r="E64" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="F64" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F64">
-        <v>162</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>683</v>
@@ -4325,14 +4330,14 @@
       <c r="C65" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="D65" s="12" t="s">
+      <c r="D65" s="8">
+        <v>162</v>
+      </c>
+      <c r="E65" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="F65" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F65">
-        <v>162</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>683</v>
@@ -4351,14 +4356,14 @@
       <c r="C66" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="8">
+        <v>162</v>
+      </c>
+      <c r="E66" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E66" s="10" t="s">
+      <c r="F66" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F66">
-        <v>162</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>683</v>
@@ -4377,14 +4382,14 @@
       <c r="C67" s="2" t="s">
         <v>549</v>
       </c>
-      <c r="D67" s="12" t="s">
+      <c r="D67" s="8">
+        <v>162</v>
+      </c>
+      <c r="E67" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="F67" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F67">
-        <v>162</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>683</v>
@@ -4403,14 +4408,14 @@
       <c r="C68" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D68" s="8">
+        <v>162</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="F68" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F68">
-        <v>162</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>683</v>
@@ -4429,14 +4434,14 @@
       <c r="C69" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="D69" s="12" t="s">
+      <c r="D69" s="8">
+        <v>162</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="F69" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F69">
-        <v>162</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>683</v>
@@ -4455,14 +4460,14 @@
       <c r="C70" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="D70" s="12" t="s">
+      <c r="D70" s="8">
+        <v>162</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="F70" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F70">
-        <v>162</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>683</v>
@@ -4481,14 +4486,14 @@
       <c r="C71" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="D71" s="12" t="s">
+      <c r="D71" s="8">
+        <v>162</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E71" s="10" t="s">
+      <c r="F71" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F71">
-        <v>162</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>683</v>
@@ -4507,14 +4512,14 @@
       <c r="C72" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D72" s="8">
+        <v>162</v>
+      </c>
+      <c r="E72" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E72" s="10" t="s">
+      <c r="F72" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F72">
-        <v>162</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>683</v>
@@ -4533,14 +4538,14 @@
       <c r="C73" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="D73" s="12" t="s">
+      <c r="D73" s="8">
+        <v>162</v>
+      </c>
+      <c r="E73" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="F73" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F73">
-        <v>162</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>683</v>
@@ -4559,14 +4564,14 @@
       <c r="C74" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="D74" s="12" t="s">
+      <c r="D74" s="8">
+        <v>162</v>
+      </c>
+      <c r="E74" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="F74" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F74">
-        <v>162</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>683</v>
@@ -4585,14 +4590,14 @@
       <c r="C75" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="D75" s="12" t="s">
+      <c r="D75" s="8">
+        <v>162</v>
+      </c>
+      <c r="E75" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="F75" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F75">
-        <v>162</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>683</v>
@@ -4611,14 +4616,14 @@
       <c r="C76" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="D76" s="12" t="s">
+      <c r="D76" s="8">
+        <v>162</v>
+      </c>
+      <c r="E76" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E76" s="10" t="s">
+      <c r="F76" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F76">
-        <v>162</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>683</v>
@@ -4637,14 +4642,14 @@
       <c r="C77" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D77" s="8">
+        <v>162</v>
+      </c>
+      <c r="E77" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E77" s="10" t="s">
+      <c r="F77" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F77">
-        <v>162</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>683</v>
@@ -4663,14 +4668,14 @@
       <c r="C78" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="D78" s="12" t="s">
+      <c r="D78" s="8">
+        <v>162</v>
+      </c>
+      <c r="E78" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E78" s="10" t="s">
+      <c r="F78" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F78">
-        <v>162</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>683</v>
@@ -4689,14 +4694,14 @@
       <c r="C79" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="D79" s="12" t="s">
+      <c r="D79" s="8">
+        <v>162</v>
+      </c>
+      <c r="E79" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E79" s="10" t="s">
+      <c r="F79" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F79">
-        <v>162</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>683</v>
@@ -4715,14 +4720,14 @@
       <c r="C80" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="D80" s="12" t="s">
+      <c r="D80" s="8">
+        <v>162</v>
+      </c>
+      <c r="E80" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E80" s="10" t="s">
+      <c r="F80" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F80">
-        <v>162</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>683</v>
@@ -4741,14 +4746,14 @@
       <c r="C81" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="8">
+        <v>162</v>
+      </c>
+      <c r="E81" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E81" s="10" t="s">
+      <c r="F81" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F81">
-        <v>162</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>683</v>
@@ -4767,14 +4772,14 @@
       <c r="C82" s="2" t="s">
         <v>564</v>
       </c>
-      <c r="D82" s="12" t="s">
+      <c r="D82" s="8">
+        <v>162</v>
+      </c>
+      <c r="E82" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E82" s="10" t="s">
+      <c r="F82" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F82">
-        <v>162</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>683</v>
@@ -4793,14 +4798,14 @@
       <c r="C83" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="D83" s="12" t="s">
+      <c r="D83" s="8">
+        <v>162</v>
+      </c>
+      <c r="E83" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E83" s="10" t="s">
+      <c r="F83" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F83">
-        <v>162</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>683</v>
@@ -4819,14 +4824,14 @@
       <c r="C84" s="2" t="s">
         <v>566</v>
       </c>
-      <c r="D84" s="12" t="s">
+      <c r="D84" s="8">
+        <v>162</v>
+      </c>
+      <c r="E84" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E84" s="10" t="s">
+      <c r="F84" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F84">
-        <v>162</v>
       </c>
       <c r="G84" s="13" t="s">
         <v>683</v>
@@ -4845,14 +4850,14 @@
       <c r="C85" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="D85" s="12" t="s">
+      <c r="D85" s="8">
+        <v>162</v>
+      </c>
+      <c r="E85" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E85" s="10" t="s">
+      <c r="F85" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F85">
-        <v>162</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>683</v>
@@ -4871,14 +4876,14 @@
       <c r="C86" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="D86" s="12" t="s">
+      <c r="D86" s="8">
+        <v>162</v>
+      </c>
+      <c r="E86" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E86" s="10" t="s">
+      <c r="F86" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F86">
-        <v>162</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>683</v>
@@ -4897,14 +4902,14 @@
       <c r="C87" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="D87" s="12" t="s">
+      <c r="D87" s="8">
+        <v>162</v>
+      </c>
+      <c r="E87" s="12" t="s">
         <v>621</v>
       </c>
-      <c r="E87" s="10" t="s">
+      <c r="F87" s="10" t="s">
         <v>676</v>
-      </c>
-      <c r="F87">
-        <v>162</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>683</v>
@@ -4934,12 +4939,12 @@
       <c r="C89" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="D89" s="16"/>
-      <c r="E89" s="10" t="s">
+      <c r="D89" s="8">
+        <v>129</v>
+      </c>
+      <c r="E89" s="16"/>
+      <c r="F89" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F89">
-        <v>129</v>
       </c>
       <c r="G89" s="12" t="s">
         <v>687</v>
@@ -4958,14 +4963,14 @@
       <c r="C90" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="D90" s="12" t="s">
+      <c r="D90" s="8">
+        <v>129</v>
+      </c>
+      <c r="E90" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E90" s="10" t="s">
+      <c r="F90" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F90">
-        <v>129</v>
       </c>
       <c r="G90" s="12" t="s">
         <v>687</v>
@@ -4984,14 +4989,14 @@
       <c r="C91" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="D91" s="12" t="s">
+      <c r="D91" s="8">
+        <v>129</v>
+      </c>
+      <c r="E91" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E91" s="10" t="s">
+      <c r="F91" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F91" s="8">
-        <v>129</v>
       </c>
       <c r="G91" s="12" t="s">
         <v>687</v>
@@ -5010,14 +5015,14 @@
       <c r="C92" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="D92" s="12" t="s">
+      <c r="D92" s="8">
+        <v>129</v>
+      </c>
+      <c r="E92" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E92" s="10" t="s">
+      <c r="F92" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F92" s="8">
-        <v>129</v>
       </c>
       <c r="G92" s="12" t="s">
         <v>687</v>
@@ -5036,14 +5041,14 @@
       <c r="C93" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="D93" s="12" t="s">
+      <c r="D93" s="8">
+        <v>129</v>
+      </c>
+      <c r="E93" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E93" s="10" t="s">
+      <c r="F93" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F93" s="8">
-        <v>129</v>
       </c>
       <c r="G93" s="12" t="s">
         <v>687</v>
@@ -5062,14 +5067,14 @@
       <c r="C94" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="D94" s="12" t="s">
+      <c r="D94" s="8">
+        <v>129</v>
+      </c>
+      <c r="E94" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E94" s="10" t="s">
+      <c r="F94" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F94" s="8">
-        <v>129</v>
       </c>
       <c r="G94" s="12" t="s">
         <v>687</v>
@@ -5088,14 +5093,14 @@
       <c r="C95" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="D95" s="12" t="s">
+      <c r="D95" s="8">
+        <v>129</v>
+      </c>
+      <c r="E95" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E95" s="10" t="s">
+      <c r="F95" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F95" s="8">
-        <v>129</v>
       </c>
       <c r="G95" s="12" t="s">
         <v>687</v>
@@ -5114,14 +5119,14 @@
       <c r="C96" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="D96" s="12" t="s">
+      <c r="D96" s="8">
+        <v>129</v>
+      </c>
+      <c r="E96" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E96" s="10" t="s">
+      <c r="F96" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F96" s="8">
-        <v>129</v>
       </c>
       <c r="G96" s="12" t="s">
         <v>687</v>
@@ -5140,14 +5145,14 @@
       <c r="C97" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="D97" s="12" t="s">
+      <c r="D97" s="8">
+        <v>129</v>
+      </c>
+      <c r="E97" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E97" s="10" t="s">
+      <c r="F97" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F97" s="8">
-        <v>129</v>
       </c>
       <c r="G97" s="12" t="s">
         <v>687</v>
@@ -5166,14 +5171,14 @@
       <c r="C98" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="D98" s="12" t="s">
+      <c r="D98" s="8">
+        <v>129</v>
+      </c>
+      <c r="E98" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E98" s="10" t="s">
+      <c r="F98" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F98" s="8">
-        <v>129</v>
       </c>
       <c r="G98" s="12" t="s">
         <v>687</v>
@@ -5192,14 +5197,14 @@
       <c r="C99" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="D99" s="12" t="s">
+      <c r="D99" s="8">
+        <v>129</v>
+      </c>
+      <c r="E99" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E99" s="10" t="s">
+      <c r="F99" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F99" s="8">
-        <v>129</v>
       </c>
       <c r="G99" s="12" t="s">
         <v>687</v>
@@ -5218,14 +5223,14 @@
       <c r="C100" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="D100" s="12" t="s">
+      <c r="D100" s="8">
+        <v>129</v>
+      </c>
+      <c r="E100" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E100" s="10" t="s">
+      <c r="F100" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F100" s="8">
-        <v>129</v>
       </c>
       <c r="G100" s="12" t="s">
         <v>687</v>
@@ -5244,14 +5249,14 @@
       <c r="C101" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="D101" s="12" t="s">
+      <c r="D101" s="8">
+        <v>129</v>
+      </c>
+      <c r="E101" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E101" s="10" t="s">
+      <c r="F101" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F101" s="8">
-        <v>129</v>
       </c>
       <c r="G101" s="12" t="s">
         <v>687</v>
@@ -5270,14 +5275,14 @@
       <c r="C102" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="D102" s="12" t="s">
+      <c r="D102" s="8">
+        <v>129</v>
+      </c>
+      <c r="E102" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E102" s="10" t="s">
+      <c r="F102" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F102" s="8">
-        <v>129</v>
       </c>
       <c r="G102" s="12" t="s">
         <v>687</v>
@@ -5296,14 +5301,14 @@
       <c r="C103" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="D103" s="12" t="s">
+      <c r="D103" s="8">
+        <v>139</v>
+      </c>
+      <c r="E103" s="12" t="s">
         <v>615</v>
       </c>
-      <c r="E103" s="10" t="s">
+      <c r="F103" s="10" t="s">
         <v>679</v>
-      </c>
-      <c r="F103" s="8">
-        <v>139</v>
       </c>
       <c r="G103" s="12" t="s">
         <v>687</v>
@@ -5333,14 +5338,14 @@
       <c r="C105" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="D105" s="12" t="s">
+      <c r="D105" s="8">
+        <v>111</v>
+      </c>
+      <c r="E105" s="12" t="s">
         <v>650</v>
       </c>
-      <c r="E105" s="10" t="s">
+      <c r="F105" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F105">
-        <v>111</v>
       </c>
       <c r="G105" s="13" t="s">
         <v>683</v>
@@ -5359,14 +5364,14 @@
       <c r="C106" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="D106" s="12" t="s">
+      <c r="D106" s="8">
+        <v>111</v>
+      </c>
+      <c r="E106" s="12" t="s">
         <v>651</v>
       </c>
-      <c r="E106" s="10" t="s">
+      <c r="F106" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F106">
-        <v>111</v>
       </c>
       <c r="G106" s="13" t="s">
         <v>683</v>
@@ -5385,14 +5390,14 @@
       <c r="C107" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="D107" s="12" t="s">
+      <c r="D107" s="8">
+        <v>111</v>
+      </c>
+      <c r="E107" s="12" t="s">
         <v>652</v>
       </c>
-      <c r="E107" s="10" t="s">
+      <c r="F107" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F107">
-        <v>111</v>
       </c>
       <c r="G107" s="13" t="s">
         <v>683</v>
@@ -5411,14 +5416,14 @@
       <c r="C108" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="D108" s="12" t="s">
+      <c r="D108" s="8">
+        <v>111</v>
+      </c>
+      <c r="E108" s="12" t="s">
         <v>653</v>
       </c>
-      <c r="E108" s="10" t="s">
+      <c r="F108" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F108">
-        <v>111</v>
       </c>
       <c r="G108" s="13" t="s">
         <v>683</v>
@@ -5437,14 +5442,14 @@
       <c r="C109" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="D109" s="12" t="s">
+      <c r="D109" s="8">
+        <v>111</v>
+      </c>
+      <c r="E109" s="12" t="s">
         <v>654</v>
       </c>
-      <c r="E109" s="10" t="s">
+      <c r="F109" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F109">
-        <v>111</v>
       </c>
       <c r="G109" s="13" t="s">
         <v>683</v>
@@ -5463,14 +5468,14 @@
       <c r="C110" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="D110" s="12" t="s">
+      <c r="D110" s="8">
+        <v>111</v>
+      </c>
+      <c r="E110" s="12" t="s">
         <v>655</v>
       </c>
-      <c r="E110" s="10" t="s">
+      <c r="F110" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F110">
-        <v>111</v>
       </c>
       <c r="G110" s="13" t="s">
         <v>683</v>
@@ -5489,14 +5494,14 @@
       <c r="C111" s="2" t="s">
         <v>590</v>
       </c>
-      <c r="D111" s="12" t="s">
+      <c r="D111" s="8">
+        <v>111</v>
+      </c>
+      <c r="E111" s="12" t="s">
         <v>656</v>
       </c>
-      <c r="E111" s="10" t="s">
+      <c r="F111" s="10" t="s">
         <v>668</v>
-      </c>
-      <c r="F111">
-        <v>111</v>
       </c>
       <c r="G111" s="13" t="s">
         <v>683</v>
@@ -5526,14 +5531,14 @@
       <c r="C113" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="D113" s="12" t="s">
+      <c r="D113" s="8">
+        <v>131</v>
+      </c>
+      <c r="E113" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="E113" s="10" t="s">
+      <c r="F113" s="10" t="s">
         <v>680</v>
-      </c>
-      <c r="F113">
-        <v>131</v>
       </c>
       <c r="G113" s="12" t="s">
         <v>688</v>
@@ -5552,14 +5557,14 @@
       <c r="C114" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="D114" s="12" t="s">
+      <c r="D114" s="8">
+        <v>131</v>
+      </c>
+      <c r="E114" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="E114" s="10" t="s">
+      <c r="F114" s="10" t="s">
         <v>680</v>
-      </c>
-      <c r="F114" s="8">
-        <v>131</v>
       </c>
       <c r="G114" s="12" t="s">
         <v>688</v>
@@ -5578,14 +5583,14 @@
       <c r="C115" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="D115" s="12" t="s">
+      <c r="D115" s="8">
+        <v>131</v>
+      </c>
+      <c r="E115" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="E115" s="10" t="s">
+      <c r="F115" s="10" t="s">
         <v>680</v>
-      </c>
-      <c r="F115" s="8">
-        <v>131</v>
       </c>
       <c r="G115" s="12" t="s">
         <v>688</v>
@@ -5604,14 +5609,14 @@
       <c r="C116" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="D116" s="12" t="s">
+      <c r="D116" s="8">
+        <v>131</v>
+      </c>
+      <c r="E116" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="E116" s="10" t="s">
+      <c r="F116" s="10" t="s">
         <v>680</v>
-      </c>
-      <c r="F116" s="8">
-        <v>131</v>
       </c>
       <c r="G116" s="12" t="s">
         <v>688</v>
@@ -5641,14 +5646,14 @@
       <c r="C118" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="D118" s="12" t="s">
+      <c r="D118" s="18">
+        <v>99</v>
+      </c>
+      <c r="E118" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="E118" s="10" t="s">
+      <c r="F118" s="10" t="s">
         <v>669</v>
-      </c>
-      <c r="F118" s="18">
-        <v>99</v>
       </c>
       <c r="G118" s="13" t="s">
         <v>683</v>
@@ -5667,14 +5672,14 @@
       <c r="C119" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="D119" s="12" t="s">
+      <c r="D119" s="18">
+        <v>99</v>
+      </c>
+      <c r="E119" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="E119" s="10" t="s">
+      <c r="F119" s="10" t="s">
         <v>669</v>
-      </c>
-      <c r="F119" s="18">
-        <v>99</v>
       </c>
       <c r="G119" s="13" t="s">
         <v>683</v>
@@ -5704,14 +5709,14 @@
       <c r="C121" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="D121" s="12" t="s">
+      <c r="D121" s="8">
+        <v>117</v>
+      </c>
+      <c r="E121" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E121" s="10" t="s">
+      <c r="F121" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F121">
-        <v>117</v>
       </c>
       <c r="G121" s="12" t="s">
         <v>689</v>
@@ -5730,14 +5735,14 @@
       <c r="C122" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="D122" s="12" t="s">
+      <c r="D122" s="8">
+        <v>117</v>
+      </c>
+      <c r="E122" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E122" s="10" t="s">
+      <c r="F122" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F122">
-        <v>117</v>
       </c>
       <c r="G122" s="12" t="s">
         <v>689</v>
@@ -5756,14 +5761,14 @@
       <c r="C123" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="D123" s="12" t="s">
+      <c r="D123" s="8">
+        <v>117</v>
+      </c>
+      <c r="E123" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E123" s="10" t="s">
+      <c r="F123" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F123">
-        <v>117</v>
       </c>
       <c r="G123" s="12" t="s">
         <v>689</v>
@@ -5782,14 +5787,14 @@
       <c r="C124" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="D124" s="12" t="s">
+      <c r="D124" s="8">
+        <v>117</v>
+      </c>
+      <c r="E124" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E124" s="10" t="s">
+      <c r="F124" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F124">
-        <v>117</v>
       </c>
       <c r="G124" s="12" t="s">
         <v>689</v>
@@ -5808,14 +5813,14 @@
       <c r="C125" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="D125" s="12" t="s">
+      <c r="D125" s="8">
+        <v>117</v>
+      </c>
+      <c r="E125" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E125" s="10" t="s">
+      <c r="F125" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F125">
-        <v>117</v>
       </c>
       <c r="G125" s="12" t="s">
         <v>689</v>
@@ -5834,14 +5839,14 @@
       <c r="C126" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="D126" s="12" t="s">
+      <c r="D126" s="8">
+        <v>117</v>
+      </c>
+      <c r="E126" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E126" s="10" t="s">
+      <c r="F126" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F126">
-        <v>117</v>
       </c>
       <c r="G126" s="12" t="s">
         <v>689</v>
@@ -5860,14 +5865,14 @@
       <c r="C127" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="D127" s="12" t="s">
+      <c r="D127" s="8">
+        <v>117</v>
+      </c>
+      <c r="E127" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E127" s="10" t="s">
+      <c r="F127" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F127">
-        <v>117</v>
       </c>
       <c r="G127" s="12" t="s">
         <v>689</v>
@@ -5886,14 +5891,14 @@
       <c r="C128" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="D128" s="12" t="s">
+      <c r="D128" s="8">
+        <v>117</v>
+      </c>
+      <c r="E128" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E128" s="10" t="s">
+      <c r="F128" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F128">
-        <v>117</v>
       </c>
       <c r="G128" s="12" t="s">
         <v>689</v>
@@ -5912,14 +5917,14 @@
       <c r="C129" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="D129" s="12" t="s">
+      <c r="D129" s="8">
+        <v>117</v>
+      </c>
+      <c r="E129" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E129" s="10" t="s">
+      <c r="F129" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F129">
-        <v>117</v>
       </c>
       <c r="G129" s="12" t="s">
         <v>689</v>
@@ -5938,14 +5943,14 @@
       <c r="C130" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="D130" s="12" t="s">
+      <c r="D130" s="8">
+        <v>117</v>
+      </c>
+      <c r="E130" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E130" s="10" t="s">
+      <c r="F130" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F130">
-        <v>117</v>
       </c>
       <c r="G130" s="12" t="s">
         <v>689</v>
@@ -5964,14 +5969,14 @@
       <c r="C131" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="D131" s="12" t="s">
+      <c r="D131" s="8">
+        <v>117</v>
+      </c>
+      <c r="E131" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E131" s="10" t="s">
+      <c r="F131" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F131">
-        <v>117</v>
       </c>
       <c r="G131" s="12" t="s">
         <v>689</v>
@@ -5990,14 +5995,14 @@
       <c r="C132" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="D132" s="12" t="s">
+      <c r="D132" s="8">
+        <v>117</v>
+      </c>
+      <c r="E132" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E132" s="10" t="s">
+      <c r="F132" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F132">
-        <v>117</v>
       </c>
       <c r="G132" s="12" t="s">
         <v>689</v>
@@ -6016,14 +6021,14 @@
       <c r="C133" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="D133" s="12" t="s">
+      <c r="D133" s="8">
+        <v>117</v>
+      </c>
+      <c r="E133" s="12" t="s">
         <v>623</v>
       </c>
-      <c r="E133" s="10" t="s">
+      <c r="F133" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F133">
-        <v>117</v>
       </c>
       <c r="G133" s="12" t="s">
         <v>689</v>
@@ -6042,14 +6047,14 @@
       <c r="C134" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="D134" s="12" t="s">
+      <c r="D134" s="8">
+        <v>95</v>
+      </c>
+      <c r="E134" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="E134" s="10" t="s">
+      <c r="F134" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F134">
-        <v>95</v>
       </c>
       <c r="G134" s="12" t="s">
         <v>689</v>
@@ -6068,14 +6073,14 @@
       <c r="C135" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="D135" s="12" t="s">
+      <c r="D135" s="8">
+        <v>95</v>
+      </c>
+      <c r="E135" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="E135" s="10" t="s">
+      <c r="F135" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F135">
-        <v>95</v>
       </c>
       <c r="G135" s="12" t="s">
         <v>689</v>
@@ -6094,14 +6099,14 @@
       <c r="C136" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="D136" s="12" t="s">
+      <c r="D136" s="8">
+        <v>95</v>
+      </c>
+      <c r="E136" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="E136" s="10" t="s">
+      <c r="F136" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F136">
-        <v>95</v>
       </c>
       <c r="G136" s="12" t="s">
         <v>689</v>
@@ -6120,14 +6125,14 @@
       <c r="C137" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="D137" s="12" t="s">
+      <c r="D137" s="8">
+        <v>95</v>
+      </c>
+      <c r="E137" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="E137" s="10" t="s">
+      <c r="F137" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F137">
-        <v>95</v>
       </c>
       <c r="G137" s="12" t="s">
         <v>689</v>
@@ -6146,14 +6151,14 @@
       <c r="C138" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="D138" s="12" t="s">
+      <c r="D138" s="8">
+        <v>95</v>
+      </c>
+      <c r="E138" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="E138" s="10" t="s">
+      <c r="F138" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F138">
-        <v>95</v>
       </c>
       <c r="G138" s="12" t="s">
         <v>689</v>
@@ -6172,14 +6177,14 @@
       <c r="C139" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="D139" s="12" t="s">
+      <c r="D139" s="8">
+        <v>95</v>
+      </c>
+      <c r="E139" s="12" t="s">
         <v>624</v>
       </c>
-      <c r="E139" s="10" t="s">
+      <c r="F139" s="10" t="s">
         <v>681</v>
-      </c>
-      <c r="F139">
-        <v>95</v>
       </c>
       <c r="G139" s="12" t="s">
         <v>689</v>
@@ -6209,14 +6214,14 @@
       <c r="C141" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="D141" s="12" t="s">
+      <c r="D141" s="8">
+        <v>84</v>
+      </c>
+      <c r="E141" s="12" t="s">
         <v>625</v>
       </c>
-      <c r="E141" s="10" t="s">
+      <c r="F141" s="10" t="s">
         <v>670</v>
-      </c>
-      <c r="F141">
-        <v>84</v>
       </c>
       <c r="G141" s="13" t="s">
         <v>683</v>
@@ -6235,14 +6240,14 @@
       <c r="C142" s="3" t="s">
         <v>468</v>
       </c>
-      <c r="D142" s="12" t="s">
+      <c r="D142" s="8">
+        <v>84</v>
+      </c>
+      <c r="E142" s="12" t="s">
         <v>626</v>
       </c>
-      <c r="E142" s="10" t="s">
+      <c r="F142" s="10" t="s">
         <v>670</v>
-      </c>
-      <c r="F142">
-        <v>84</v>
       </c>
       <c r="G142" s="13" t="s">
         <v>683</v>
@@ -6261,14 +6266,14 @@
       <c r="C143" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="D143" s="12" t="s">
+      <c r="D143" s="8">
+        <v>84</v>
+      </c>
+      <c r="E143" s="12" t="s">
         <v>627</v>
       </c>
-      <c r="E143" s="10" t="s">
+      <c r="F143" s="10" t="s">
         <v>670</v>
-      </c>
-      <c r="F143">
-        <v>84</v>
       </c>
       <c r="G143" s="13" t="s">
         <v>683</v>
@@ -6287,14 +6292,14 @@
       <c r="C144" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="D144" s="12" t="s">
+      <c r="D144" s="8">
+        <v>84</v>
+      </c>
+      <c r="E144" s="12" t="s">
         <v>628</v>
       </c>
-      <c r="E144" s="10" t="s">
+      <c r="F144" s="10" t="s">
         <v>670</v>
-      </c>
-      <c r="F144">
-        <v>84</v>
       </c>
       <c r="G144" s="13" t="s">
         <v>683</v>
@@ -6313,14 +6318,14 @@
       <c r="C145" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="D145" s="12" t="s">
+      <c r="D145" s="8">
+        <v>84</v>
+      </c>
+      <c r="E145" s="12" t="s">
         <v>629</v>
       </c>
-      <c r="E145" s="10" t="s">
+      <c r="F145" s="10" t="s">
         <v>670</v>
-      </c>
-      <c r="F145">
-        <v>84</v>
       </c>
       <c r="G145" s="13" t="s">
         <v>683</v>
@@ -6339,14 +6344,14 @@
       <c r="C146" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="D146" s="12" t="s">
+      <c r="D146" s="8">
+        <v>84</v>
+      </c>
+      <c r="E146" s="12" t="s">
         <v>630</v>
       </c>
-      <c r="E146" s="10" t="s">
+      <c r="F146" s="10" t="s">
         <v>670</v>
-      </c>
-      <c r="F146">
-        <v>84</v>
       </c>
       <c r="G146" s="13" t="s">
         <v>683</v>
@@ -6376,14 +6381,14 @@
       <c r="C148" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="D148" s="11" t="s">
+      <c r="D148" s="8">
+        <v>150</v>
+      </c>
+      <c r="E148" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E148" s="10" t="s">
+      <c r="F148" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F148">
-        <v>150</v>
       </c>
       <c r="G148" s="12" t="s">
         <v>690</v>
@@ -6402,14 +6407,14 @@
       <c r="C149" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="D149" s="11" t="s">
+      <c r="D149" s="8">
+        <v>150</v>
+      </c>
+      <c r="E149" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E149" s="10" t="s">
+      <c r="F149" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F149">
-        <v>150</v>
       </c>
       <c r="G149" s="12" t="s">
         <v>690</v>
@@ -6428,14 +6433,14 @@
       <c r="C150" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="D150" s="11" t="s">
+      <c r="D150" s="8">
+        <v>150</v>
+      </c>
+      <c r="E150" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E150" s="10" t="s">
+      <c r="F150" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F150">
-        <v>150</v>
       </c>
       <c r="G150" s="12" t="s">
         <v>690</v>
@@ -6454,14 +6459,14 @@
       <c r="C151" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="D151" s="11" t="s">
+      <c r="D151" s="8">
+        <v>150</v>
+      </c>
+      <c r="E151" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E151" s="10" t="s">
+      <c r="F151" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F151">
-        <v>150</v>
       </c>
       <c r="G151" s="12" t="s">
         <v>690</v>
@@ -6480,14 +6485,14 @@
       <c r="C152" s="3" t="s">
         <v>477</v>
       </c>
-      <c r="D152" s="11" t="s">
+      <c r="D152" s="8">
+        <v>150</v>
+      </c>
+      <c r="E152" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E152" s="10" t="s">
+      <c r="F152" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F152">
-        <v>150</v>
       </c>
       <c r="G152" s="12" t="s">
         <v>690</v>
@@ -6506,14 +6511,14 @@
       <c r="C153" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="D153" s="11" t="s">
+      <c r="D153" s="8">
+        <v>150</v>
+      </c>
+      <c r="E153" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E153" s="10" t="s">
+      <c r="F153" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F153">
-        <v>150</v>
       </c>
       <c r="G153" s="12" t="s">
         <v>690</v>
@@ -6532,14 +6537,14 @@
       <c r="C154" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="D154" s="11" t="s">
+      <c r="D154" s="8">
+        <v>150</v>
+      </c>
+      <c r="E154" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E154" s="10" t="s">
+      <c r="F154" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F154">
-        <v>150</v>
       </c>
       <c r="G154" s="12" t="s">
         <v>690</v>
@@ -6558,14 +6563,14 @@
       <c r="C155" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="D155" s="11" t="s">
+      <c r="D155" s="8">
+        <v>150</v>
+      </c>
+      <c r="E155" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E155" s="10" t="s">
+      <c r="F155" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F155">
-        <v>150</v>
       </c>
       <c r="G155" s="12" t="s">
         <v>690</v>
@@ -6584,14 +6589,14 @@
       <c r="C156" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="D156" s="11" t="s">
+      <c r="D156" s="8">
+        <v>150</v>
+      </c>
+      <c r="E156" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E156" s="10" t="s">
+      <c r="F156" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F156">
-        <v>150</v>
       </c>
       <c r="G156" s="12" t="s">
         <v>690</v>
@@ -6610,14 +6615,14 @@
       <c r="C157" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="D157" s="11" t="s">
+      <c r="D157" s="8">
+        <v>150</v>
+      </c>
+      <c r="E157" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="E157" s="10" t="s">
+      <c r="F157" s="10" t="s">
         <v>671</v>
-      </c>
-      <c r="F157">
-        <v>150</v>
       </c>
       <c r="G157" s="12" t="s">
         <v>690</v>
@@ -6647,14 +6652,14 @@
       <c r="C159" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="D159" s="11" t="s">
+      <c r="D159" s="8">
+        <v>209</v>
+      </c>
+      <c r="E159" s="11" t="s">
         <v>632</v>
       </c>
-      <c r="E159" s="10" t="s">
+      <c r="F159" s="10" t="s">
         <v>672</v>
-      </c>
-      <c r="F159">
-        <v>209</v>
       </c>
       <c r="G159" s="12" t="s">
         <v>691</v>
@@ -6673,14 +6678,14 @@
       <c r="C160" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="D160" s="11" t="s">
+      <c r="D160" s="8">
+        <v>209</v>
+      </c>
+      <c r="E160" s="11" t="s">
         <v>632</v>
       </c>
-      <c r="E160" s="10" t="s">
+      <c r="F160" s="10" t="s">
         <v>672</v>
-      </c>
-      <c r="F160">
-        <v>209</v>
       </c>
       <c r="G160" s="12" t="s">
         <v>691</v>
@@ -6699,14 +6704,14 @@
       <c r="C161" s="3" t="s">
         <v>506</v>
       </c>
-      <c r="D161" s="11" t="s">
+      <c r="D161" s="8">
+        <v>475</v>
+      </c>
+      <c r="E161" s="11" t="s">
         <v>633</v>
       </c>
-      <c r="E161" s="17" t="s">
+      <c r="F161" s="17" t="s">
         <v>682</v>
-      </c>
-      <c r="F161" s="8">
-        <v>475</v>
       </c>
       <c r="G161" s="12" t="s">
         <v>692</v>
@@ -6725,14 +6730,14 @@
       <c r="C162" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="D162" s="11" t="s">
+      <c r="D162" s="18">
+        <v>475</v>
+      </c>
+      <c r="E162" s="11" t="s">
         <v>633</v>
       </c>
-      <c r="E162" s="10" t="s">
+      <c r="F162" s="10" t="s">
         <v>682</v>
-      </c>
-      <c r="F162" s="18">
-        <v>475</v>
       </c>
       <c r="G162" s="12" t="s">
         <v>692</v>
@@ -6745,8 +6750,7 @@
     <row r="170" spans="1:9">
       <c r="B170" s="8"/>
       <c r="C170" s="8"/>
-      <c r="D170" s="8"/>
-      <c r="F170" s="8"/>
+      <c r="E170" s="8"/>
       <c r="G170" s="8"/>
       <c r="H170" s="8"/>
       <c r="I170" s="8"/>
@@ -6754,8 +6758,7 @@
     <row r="171" spans="1:9">
       <c r="B171" s="8"/>
       <c r="C171" s="8"/>
-      <c r="D171" s="8"/>
-      <c r="F171" s="8"/>
+      <c r="E171" s="8"/>
       <c r="G171" s="8"/>
       <c r="H171" s="8"/>
       <c r="I171" s="8"/>
@@ -6763,8 +6766,7 @@
     <row r="172" spans="1:9">
       <c r="B172" s="8"/>
       <c r="C172" s="8"/>
-      <c r="D172" s="8"/>
-      <c r="F172" s="8"/>
+      <c r="E172" s="8"/>
       <c r="G172" s="8"/>
       <c r="H172" s="8"/>
       <c r="I172" s="8"/>
@@ -6772,8 +6774,7 @@
     <row r="173" spans="1:9">
       <c r="B173" s="8"/>
       <c r="C173" s="8"/>
-      <c r="D173" s="8"/>
-      <c r="F173" s="8"/>
+      <c r="E173" s="8"/>
       <c r="G173" s="8"/>
       <c r="H173" s="8"/>
       <c r="I173" s="8"/>
@@ -6781,8 +6782,7 @@
     <row r="174" spans="1:9">
       <c r="B174" s="8"/>
       <c r="C174" s="8"/>
-      <c r="D174" s="8"/>
-      <c r="F174" s="8"/>
+      <c r="E174" s="8"/>
       <c r="G174" s="8"/>
       <c r="H174" s="8"/>
       <c r="I174" s="8"/>
@@ -6790,8 +6790,7 @@
     <row r="175" spans="1:9">
       <c r="B175" s="8"/>
       <c r="C175" s="8"/>
-      <c r="D175" s="8"/>
-      <c r="F175" s="8"/>
+      <c r="E175" s="8"/>
       <c r="G175" s="8"/>
       <c r="H175" s="8"/>
       <c r="I175" s="8"/>
@@ -6799,8 +6798,7 @@
     <row r="176" spans="1:9">
       <c r="B176" s="8"/>
       <c r="C176" s="8"/>
-      <c r="D176" s="8"/>
-      <c r="F176" s="8"/>
+      <c r="E176" s="8"/>
       <c r="G176" s="8"/>
       <c r="H176" s="8"/>
       <c r="I176" s="8"/>
@@ -6808,8 +6806,7 @@
     <row r="177" spans="2:9">
       <c r="B177" s="8"/>
       <c r="C177" s="8"/>
-      <c r="D177" s="8"/>
-      <c r="F177" s="8"/>
+      <c r="E177" s="8"/>
       <c r="G177" s="8"/>
       <c r="H177" s="8"/>
       <c r="I177" s="8"/>
@@ -6817,8 +6814,7 @@
     <row r="178" spans="2:9">
       <c r="B178" s="8"/>
       <c r="C178" s="8"/>
-      <c r="D178" s="8"/>
-      <c r="F178" s="8"/>
+      <c r="E178" s="8"/>
       <c r="G178" s="8"/>
       <c r="H178" s="8"/>
       <c r="I178" s="8"/>
@@ -6826,8 +6822,7 @@
     <row r="179" spans="2:9">
       <c r="B179" s="8"/>
       <c r="C179" s="8"/>
-      <c r="D179" s="8"/>
-      <c r="F179" s="8"/>
+      <c r="E179" s="8"/>
       <c r="G179" s="8"/>
       <c r="H179" s="8"/>
       <c r="I179" s="8"/>
@@ -6835,8 +6830,7 @@
     <row r="180" spans="2:9">
       <c r="B180" s="8"/>
       <c r="C180" s="8"/>
-      <c r="D180" s="8"/>
-      <c r="F180" s="8"/>
+      <c r="E180" s="8"/>
       <c r="G180" s="8"/>
       <c r="H180" s="8"/>
       <c r="I180" s="8"/>

</xml_diff>